<commit_message>
se agrego productos eufar
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="123">
   <si>
     <t>id</t>
   </si>
@@ -108,6 +108,331 @@
     <t>https://res.cloudinary.com/diqmtzief/image/upload/v1731095332/tnW0NfBg_uffal6.png</t>
   </si>
   <si>
+    <t>Detergente Multienzimático Bonzyme</t>
+  </si>
+  <si>
+    <t>Disponible en presentaciones de 90ml, 1 litro, galón y 5 litros.
+El Detergente Multienzimático Bonzyme es una solución concentrada diseñada para la limpieza profunda de instrumentos odontológicos y médicos. Su fórmula contiene múltiples enzimas que descomponen eficazmente residuos orgánicos como sangre, proteínas y tejidos, facilitando la esterilización completa. Es una herramienta esencial para mantener un alto estándar de higiene y prevenir infecciones en entornos clínicos.</t>
+  </si>
+  <si>
+    <t>Fórmula multienzimática que asegura una limpieza profunda.
+Compatible con acero inoxidable, vidrio y otros materiales de instrumental clínico.
+Biodegradable y seguro para el medio ambiente.
+Disponible en diferentes presentaciones para adaptarse a las necesidades del consultorio.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732220634/45oFikcw_rubfc6.png</t>
+  </si>
+  <si>
+    <t>Alvofar Plus Pote x 10 gr</t>
+  </si>
+  <si>
+    <t>El Alvofar Plus es un material terapéutico diseñado para el tratamiento de alveolitis y la protección de cavidades post-extracción dental. Su fórmula avanzada alivia el dolor, controla la inflamación y acelera el proceso de cicatrización. Este producto es ampliamente utilizado en odontología por su eficacia en el manejo de complicaciones postquirúrgicas, proporcionando comodidad y rápida recuperación a los pacientes.</t>
+  </si>
+  <si>
+    <t>Presentación en pote de 10g, ideal para múltiples aplicaciones.
+Formulación especializada para el manejo de alveolitis.
+Efecto analgésico, antiinflamatorio y cicatrizante.
+Fácil aplicación directa en la cavidad post-extracción.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732219502/-iCaqnbA_zeh3wm.png</t>
+  </si>
+  <si>
+    <t>Acido Fluorhídrico 9.6%</t>
+  </si>
+  <si>
+    <t>El Ácido Fluorhídrico 9.6% de Eufar es un agente químico utilizado en odontología para el grabado de porcelanas y cerámicas dentales. Este producto prepara las superficies cerámicas para mejorar la adhesión de resinas compuestas y cementos adhesivos, garantizando un fuerte enlace mecánico entre el material restaurador y la superficie dental. Es un material esencial en procedimientos de odontología estética y restauradora.</t>
+  </si>
+  <si>
+    <t>Concentración del 9.6%, óptima para el grabado de porcelanas y cerámicas dentales.
+Mejora la adhesión de resinas compuestas y cementos adhesivos.
+Presentación segura y práctica para uso clínico.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732219082/S7xT5C1w_fbqhui.jpg</t>
+  </si>
+  <si>
+    <t>Jabon Bonfar Galon</t>
+  </si>
+  <si>
+    <t>El Jabón Bonfar en presentación de galón es un jabón líquido antibacterial de alta calidad, ideal para garantizar la higiene en entornos clínicos y odontológicos. Formulado para eliminar bacterias y gérmenes de manera eficaz, es una solución económica y práctica para el uso frecuente en consultorios y clínicas, promoviendo un ambiente seguro y limpio para pacientes y profesionales.</t>
+  </si>
+  <si>
+    <t>Presentación en galón (4 litros), ideal para uso continuo.
+Fórmula antibacterial que elimina gérmenes y bacterias.
+Suave con la piel, adecuado para el lavado frecuente de manos.
+Recomendado para consultorios odontológicos y entornos médicos.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732220249/EFcn0Irg_xuixjc.png</t>
+  </si>
+  <si>
+    <t>Jabon Bonfar x 500ml</t>
+  </si>
+  <si>
+    <t>El Jabón Bonfar de Eufar es un jabón líquido antibacterial especialmente formulado para garantizar una limpieza eficaz y segura en entornos clínicos. Su fórmula suave protege la piel mientras elimina bacterias y otros agentes patógenos, siendo ideal para el uso en consultorios odontológicos y áreas de atención médica. Este producto es indispensable para mantener altos estándares de higiene y prevenir infecciones cruzadas.</t>
+  </si>
+  <si>
+    <t>Presentación en envase de 500ml con dosificador para fácil aplicación.
+Fórmula antibacterial que elimina eficazmente gérmenes.
+Suave con la piel, apto para uso frecuente.
+Ideal para clínicas odontológicas y ambientes clínicos.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732220036/wLF63Rkw_lxjpw9.png</t>
+  </si>
+  <si>
+    <t>Dentofar x 5ml Desensibilizante</t>
+  </si>
+  <si>
+    <t>El Dentofar es un desensibilizante de alta eficacia diseñado para tratar la hipersensibilidad dental, proporcionando alivio rápido y duradero. Su fórmula especializada actúa bloqueando los túbulos dentinarios expuestos, reduciendo la sensibilidad al contacto con alimentos, bebidas o estímulos térmicos. Es un producto indispensable en tratamientos restaurativos y preventivos en odontología.</t>
+  </si>
+  <si>
+    <t>Presentación en frasco de 5 ml con aplicador preciso.
+Fórmula diseñada para bloquear los túbulos dentinarios.
+Proporciona alivio inmediato y duradero de la sensibilidad dental.
+Seguro y eficaz en dientes naturales y restauraciones.</t>
+  </si>
+  <si>
+    <t>Restaurativos</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732221029/snFk_1jQ_ocmmy1.png</t>
+  </si>
+  <si>
+    <t>Pasta Profilactica Detarfar Colapsible</t>
+  </si>
+  <si>
+    <t>La Pasta Profiláctica Detarfar es un producto diseñado para la limpieza y el pulido dental profesional. Con propiedades desensibilizantes, esta pasta ayuda a eliminar manchas, placa y depósitos suaves, dejando una superficie dental lisa y preparada para procedimientos posteriores. Es ideal para consultas preventivas y restaurativas.</t>
+  </si>
+  <si>
+    <t>Fórmula con propiedades desensibilizantes para mayor confort del paciente.
+Textura y grano adecuados para una limpieza eficaz sin dañar el esmalte.
+Disponible en dos presentaciones prácticas: 50g (ideal para uso específico) y 12 onzas (uso frecuente en consultorio).
+Compatible con el uso de cepillos o copas de profilaxis.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732221518/d-01fPEQ_nixdwe.png</t>
+  </si>
+  <si>
+    <t>Polvo Detarfar Prophy 120g</t>
+  </si>
+  <si>
+    <t>El Polvo Detarfar Prophy es un producto de alta calidad diseñado para procedimientos de profilaxis dental profesional. Este polvo es ideal para la limpieza profunda de manchas, placa y depósitos dentales en combinación con equipos de limpieza por aire. Su fórmula es suave con el esmalte, dejando una superficie dental perfectamente pulida y preparada para otros tratamientos.</t>
+  </si>
+  <si>
+    <t>Presentación de 120g, ideal para uso profesional en consultorios.
+Fórmula efectiva y segura para la eliminación de manchas y placa.
+Compatible con equipos de limpieza por aire y sistemas de abrasión dental.
+Textura diseñada para no dañar el esmalte ni causar molestias al paciente.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732221711/v0u25_LQ_wxrvx2.png</t>
+  </si>
+  <si>
+    <t>Revelador de Placa Ditono x 10ml</t>
+  </si>
+  <si>
+    <t>El Revelador de Placa Ditono es un producto diseñado para resaltar la presencia de placa bacteriana en los dientes, facilitando su identificación durante las consultas odontológicas o en el cuidado bucal personal. Su fórmula coloreada permite identificar áreas con mala higiene o acumulación de placa, ayudando a mejorar la técnica de cepillado y prevenir problemas dentales.</t>
+  </si>
+  <si>
+    <t>Presentación en frasco de 10ml, práctico y fácil de usar.
+Fórmula segura y efectiva que resalta la placa bacteriana con un color distintivo.
+Ideal para uso profesional en consultorios y también para la educación en higiene bucal en casa.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732221948/ycsb98wA_j7m6bm.png</t>
+  </si>
+  <si>
+    <t>Eucida Advanced x 750ml</t>
+  </si>
+  <si>
+    <t>Eucida Advanced es un desinfectante y limpiador de alta eficacia diseñado para el entorno odontológico. Su fórmula avanzada permite una limpieza profunda y desinfección de superficies, equipos e instrumentos dentales, eliminando microorganismos patógenos y garantizando un entorno clínico seguro. Ideal para la limpieza de consultorios odontológicos y de superficies que entran en contacto con pacientes.</t>
+  </si>
+  <si>
+    <t>Presentación de 750ml, ideal para uso frecuente en consultorios odontológicos.
+Eficaz contra una amplia gama de bacterias, virus y hongos.
+Producto listo para usar, sin necesidad de dilución.
+Apto para superficies duras, equipos, muebles y utensilios en consultorios dentales.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732222265/17bnYlMQ_t9ilka.png</t>
+  </si>
+  <si>
+    <t>Eugenol Eufar x 15ml</t>
+  </si>
+  <si>
+    <t>El Eugenol Eufar es un producto odontológico utilizado por su capacidad anestésica, antiinflamatoria y como material base en procedimientos restaurativos. Se emplea comúnmente en el tratamiento de dientes temporales, obturaciones provisionales y como auxiliar en el manejo de la pulpa dental. Gracias a su acción calmante y su alta efectividad, es esencial en la odontología para ofrecer comodidad al paciente durante los procedimientos.</t>
+  </si>
+  <si>
+    <t>Presentación de 15ml, adecuado para uso profesional.
+Propiedades analgésicas, lo que ayuda a reducir el dolor y la incomodidad durante tratamientos temporales.
+Ideal para mezclarse con otros materiales como óxido de zinc para crear cementos temporales o bases protectoras.
+También utilizado en la preparación de medicamentos y pastas utilizadas para la desinfección de conductos radiculares.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732222515/mW3gz_tA_gvc5iu.png</t>
+  </si>
+  <si>
+    <t>Gel Antibacterial Farben 65% x 500ml</t>
+  </si>
+  <si>
+    <t>El Gel Antibacterial Farben con un 65% de concentración de alcohol es ideal para la desinfección rápida y eficaz de las manos en entornos odontológicos y clínicos. Su formulación avanzada permite una limpieza profunda, eliminando hasta el 99.9% de los gérmenes y bacterias, sin necesidad de agua. Este gel es un indispensable en la práctica diaria de la odontología, tanto para el personal de la clínica como para los pacientes, ayudando a mantener estándares de higiene rigurosos.</t>
+  </si>
+  <si>
+    <t>Concentración de 65% de alcohol, garantizando una acción antimicrobiana efectiva.
+Presentación de 500ml, ideal para uso continuo en clínicas y consultorios odontológicos.
+Textura de gel, fácil de aplicar y de rápida absorción sin dejar residuos pegajosos.
+Higieniza y desinfecta las manos eliminando hasta el 99.9% de bacterias y virus.
+No requiere enjuague con agua, lo que permite una desinfección rápida en cualquier momento.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732222732/UaoolzRg_dniiwt.png</t>
+  </si>
+  <si>
+    <t>Fluofar Chicle</t>
+  </si>
+  <si>
+    <t>El Fluofar Chicle es un gel fluorado diseñado para la aplicación tópica en pacientes, proporcionando una protección efectiva contra las caries. Con su agradable sabor a chicle, este producto se utiliza principalmente en procedimientos odontológicos preventivos, permitiendo la remineralización del esmalte dental y la prevención de la aparición de caries.</t>
+  </si>
+  <si>
+    <t>Presentación en 240ml y 500ml, ideal para su uso en consultorios y clínicas odontológicas.
+Sabor agradable a chicle, lo que lo hace más atractivo y cómodo para los pacientes, especialmente los niños.
+Fórmula fluorinada, rica en flúor para proporcionar una protección efectiva contra las caries y fortalecer el esmalte dental.
+Producto de uso profesional: se utiliza en tratamientos de prevención y protección dental, aplicable de forma rápida y fácil en las consultas.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732222972/uRuxE_jQ_ifcfcp.png</t>
+  </si>
+  <si>
+    <t>Glutfar 2% Galon</t>
+  </si>
+  <si>
+    <t>El Glutfar 2% es un desinfectante de amplio espectro, especialmente formulado para la desinfección de superficies, equipos e instrumentos en clínicas odontológicas. Su concentración al 2% de glutaraldehído lo convierte en un potente germicida, bactericida, virucida y fungicida, ideal para la limpieza profunda en consultorios odontológicos, hospitales y clínicas.</t>
+  </si>
+  <si>
+    <t>Concentración al 2% de glutaraldehído, un potente desinfectante de amplio espectro.
+Presentación de 1 galón (3.78 L), adecuado para el uso continuo en clínicas y consultorios odontológicos.
+Eficaz contra una amplia gama de patógenos, incluyendo virus, bacterias y hongos.
+Etiqueta verde, lo que indica que está formulado para su uso en áreas clínicas y de atención a pacientes.
+Fórmula de acción rápida, ideal para la desinfección de superficies y equipos no invasivos.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732223204/uHi3SYzg_kxdo6w.png</t>
+  </si>
+  <si>
+    <t>Tirillas De Verificacion x 100 und Quantofix</t>
+  </si>
+  <si>
+    <t>Las Tirillas de Verificación Quantofix son herramientas precisas y confiables para la medición rápida de diversos parámetros en el entorno odontológico, como la presencia de compuestos o el nivel de pH. Este producto es indispensable para profesionales que necesitan realizar verificaciones rápidas y efectivas durante sus procedimientos.</t>
+  </si>
+  <si>
+    <t>Presentación de 100 tirillas, garantizando un uso prolongado y económico en clínicas odontológicas.
+Alta precisión en la medición de sustancias, proporcionando resultados rápidos y fiables.
+Fácil uso: ideal para ser empleada en cualquier procedimiento donde se necesite controlar la calidad de los compuestos utilizados o verificar la concentración de ciertos materiales.
+Versátil: adecuado para medir una amplia variedad de sustancias utilizadas en odontología.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732223412/g56X37mA_xaepyw.png</t>
+  </si>
+  <si>
+    <t>Glutfar 2% Plus HLD</t>
+  </si>
+  <si>
+    <t>El Glutfar 2% Plus HLD es una solución desinfectante de alta eficacia diseñada para la desinfección de instrumentos odontológicos y equipos médicos no invasivos. Su potente formulación con un 2% de glutaraldehído asegura una acción antimicrobiana efectiva contra bacterias, virus, hongos y esporas, lo que lo convierte en un producto indispensable para la esterilización de material odontológico en clínicas y consultorios.</t>
+  </si>
+  <si>
+    <t>Concentración de 2% de glutaraldehído: potente y eficaz contra microorganismos patógenos.
+Presentación en 5 litros, 1 litro, 500ml y galón: ideal para uso clínico con diferentes necesidades de volumen.
+Desinfección de alto nivel (HLD): asegura la eliminación de microorganismos y esporas, proporcionando seguridad en la manipulación de los instrumentos.
+Apto para la desinfección de instrumentos dentales de metal, plástico y otros materiales comunes en la práctica odontológica.
+Fórmula de acción rápida que no deja residuos tóxicos en los instrumentos.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732223741/WEM7yGdw_gdix3c.png</t>
+  </si>
+  <si>
+    <t>Cemento Grossfar 10gr</t>
+  </si>
+  <si>
+    <t>El Cemento Grossfar 10gr Eufar es un material dental de alta calidad, especialmente formulado para la fijación de restauraciones dentales como coronas, puentes, carillas y otros elementos protésicos. Su característica principal es su capacidad de adherir con firmeza y durabilidad, proporcionando un ajuste preciso y seguro.</t>
+  </si>
+  <si>
+    <t>Presentación de 10gr, ideal para varios procedimientos de fijación dental.
+Fijación fuerte y duradera: asegura una adherencia efectiva, garantizando que las restauraciones permanezcan en su lugar durante un largo período de tiempo.
+Fácil de mezclar y aplicar, lo que facilita su uso en el consultorio dental y reduce los tiempos de procedimiento.
+Resistencia al desgaste y a las cargas masticatorias, proporcionando estabilidad a largo plazo.
+Compatible con otros materiales restaurativos y adhesivos dentales.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732223939/UXMvj6pg_z8yx39.png</t>
+  </si>
+  <si>
+    <t>Hemofar x 7ml</t>
+  </si>
+  <si>
+    <t>Hemofar es un hemostático de uso odontológico, especialmente formulado para el control y manejo de hemorragias durante procedimientos dentales. Presentado en un envase de 7ml, este producto ayuda a detener rápidamente el sangrado, facilitando la realización de tratamientos sin complicaciones por sangrado excesivo.</t>
+  </si>
+  <si>
+    <t>Presentación de 7ml, ideal para ser utilizado en diversos procedimientos dentales.
+Fórmula hemostática, que actúa rápidamente sobre la zona afectada para controlar las hemorragias.
+Fácil aplicación, generalmente utilizado en áreas orales donde se presenta sangrado durante o después de un tratamiento.
+Producto estéril, garantizando la seguridad del paciente durante su uso.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732224144/l5a6I_rQ_k7rq4x.png</t>
+  </si>
+  <si>
+    <t>Momifar x 7ml</t>
+  </si>
+  <si>
+    <t>El Momifar Eufar es un desensibilizante dental de alta eficacia, formulado para aliviar la sensibilidad dental en pacientes que experimentan dolor o incomodidad debido a la exposición de las terminaciones nerviosas en los dientes. Este producto es especialmente útil durante y después de tratamientos de restauración o limpieza profunda, proporcionando un alivio inmediato y prolongado.</t>
+  </si>
+  <si>
+    <t>Presentación de 7ml, ideal para tratamientos puntuales en consultorios odontológicos.
+Eficaz contra la sensibilidad dental en pacientes, proporcionando alivio rápido tras procedimientos.
+Fórmula de fácil aplicación que actúa en pocos minutos.
+Apto para su uso en pacientes con dientes sensibles o que requieren tratamientos invasivos.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732224457/tmyjgnrg_uqgzfe.png</t>
+  </si>
+  <si>
+    <t>Oxido de Zinc x 175g</t>
+  </si>
+  <si>
+    <t>El Óxido de Zinc Eufar es un polvo de alta calidad utilizado en odontología para la preparación de cementos dentales y como componente en la fabricación de otros materiales restauradores. Es un producto esencial en la creación de mezclas para el tratamiento de cavidades y la fabricación de selladores temporales. Su alta pureza y propiedades biocompatibles lo hacen ideal para una variedad de procedimientos odontológicos.</t>
+  </si>
+  <si>
+    <t>Presentación de 175g, una cantidad ideal para su uso en clínicas odontológicas.
+Alta pureza y calidad, asegurando la efectividad en los tratamientos.
+Utilizado en la preparación de cementos dentales, material base para restauraciones y recubrimientos.
+Excelente biocompatibilidad, minimizando el riesgo de reacciones adversas en los pacientes.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732224556/MWIyIXoQ_fsq83c.png</t>
+  </si>
+  <si>
+    <t>Perifar Restaurador de Autoclave x 750ml</t>
+  </si>
+  <si>
+    <t>El Perifar Restaurador de Autoclave es una solución especializada para la limpieza, mantenimiento y restauración de equipos de esterilización, como autoclaves. Este producto es ideal para remover residuos de minerales, óxido y otras impurezas que puedan acumularse con el tiempo, prolongando la vida útil del equipo y asegurando su correcto funcionamiento.</t>
+  </si>
+  <si>
+    <t>Fórmula efectiva diseñada para limpiar y restaurar superficies internas y externas de autoclaves.
+Capacidad de 750ml, ideal para uso frecuente en clínicas y consultorios odontológicos.
+Ayuda a prevenir la acumulación de residuos de cal y minerales.
+Contribuye al mantenimiento del equipo, mejorando su rendimiento y extendiendo su vida útil.
+Producto seguro para equipos de acero inoxidable y otros materiales comunes en autoclaves.</t>
+  </si>
+  <si>
+    <t>Equipos</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732224857/zS-wQF0Q_qvfph2.png</t>
+  </si>
+  <si>
     <t>Adhesivo Prime &amp; Bond Universal</t>
   </si>
   <si>
@@ -120,20 +445,33 @@
 Presentación fácil de usar que optimiza los tiempos de aplicación</t>
   </si>
   <si>
-    <t>Accesorios</t>
-  </si>
-  <si>
     <t>Dentsply Sirona</t>
   </si>
   <si>
     <t>https://res.cloudinary.com/diqmtzief/image/upload/v1731614688/primebond-universal_o1cfsi.jpg</t>
+  </si>
+  <si>
+    <t>Resina Spectra Basic A2 Jeringa 4g</t>
+  </si>
+  <si>
+    <t>La Resina Spectra Basic A2 de Dentsply Sirona es un material de restauración dental de alta calidad diseñado para la reconstrucción estética y funcional de dientes anteriores y posteriores. Su fórmula avanzada garantiza una excelente manipulación, fácil modelado, y un acabado de alta estética, ideal para procedimientos restauradores directos. Con un tono universal A2, se adapta fácilmente al color natural del diente, asegurando resultados duraderos y estéticamente agradables.</t>
+  </si>
+  <si>
+    <t>Presentación en jeringa de 4g para aplicaciones directas y precisas.
+Tono A2 universal que se adapta a múltiples tonalidades dentales.
+Excelente resistencia mecánica y acabado brillante.
+Ideal para restauraciones en dientes anteriores y posteriores.
+Fácil de manipular, con propiedades de baja contracción.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732218579/resina-spectra-basic-jeringa.jpg_umh4ld.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -163,6 +501,22 @@
       <u/>
       <color rgb="FF0000FF"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF434343"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF434343"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -353,7 +707,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -405,6 +759,12 @@
     <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="9" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -412,12 +772,12 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="12" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -478,7 +838,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I7" displayName="Productos" name="Productos" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I29" displayName="Productos" name="Productos" id="1">
   <tableColumns count="9">
     <tableColumn name="id" id="1"/>
     <tableColumn name="nombre" id="2"/>
@@ -853,39 +1213,626 @@
       <c r="A6" s="5">
         <v>5.0</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="14" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="14" t="s">
+    </row>
+    <row r="7">
+      <c r="A7" s="9">
+        <v>6.0</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="16" t="s">
+      <c r="C7" s="11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="17"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="21"/>
+      <c r="D7" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="9">
+        <v>8.0</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="5">
+        <v>9.0</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="9">
+        <v>10.0</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="12"/>
+      <c r="I11" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="5">
+        <v>11.0</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="7"/>
+      <c r="I12" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="9">
+        <v>12.0</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="5">
+        <v>13.0</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="9">
+        <v>14.0</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="12"/>
+      <c r="I15" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="5">
+        <v>15.0</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="9">
+        <v>16.0</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="5">
+        <v>17.0</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="7"/>
+      <c r="I18" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="9">
+        <v>18.0</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="12"/>
+      <c r="I19" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="5">
+        <v>19.0</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="I20" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="9">
+        <v>20.0</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="12"/>
+      <c r="I21" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="5">
+        <v>21.0</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="I22" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="9">
+        <v>22.0</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="12"/>
+      <c r="I23" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="5">
+        <v>23.0</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="7"/>
+      <c r="I24" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="9">
+        <v>24.0</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="12"/>
+      <c r="I25" s="18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="5">
+        <v>25.0</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="9">
+        <v>26.0</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="12"/>
+      <c r="I27" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="5">
+        <v>27.0</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="7"/>
+      <c r="I28" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="19">
+        <v>28.0</v>
+      </c>
+      <c r="B29" s="20"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="23"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -894,10 +1841,32 @@
     <hyperlink r:id="rId3" ref="I4"/>
     <hyperlink r:id="rId4" ref="I5"/>
     <hyperlink r:id="rId5" ref="I6"/>
+    <hyperlink r:id="rId6" ref="I7"/>
+    <hyperlink r:id="rId7" ref="I8"/>
+    <hyperlink r:id="rId8" ref="I9"/>
+    <hyperlink r:id="rId9" ref="I10"/>
+    <hyperlink r:id="rId10" ref="I11"/>
+    <hyperlink r:id="rId11" ref="I12"/>
+    <hyperlink r:id="rId12" ref="I13"/>
+    <hyperlink r:id="rId13" ref="I14"/>
+    <hyperlink r:id="rId14" ref="I15"/>
+    <hyperlink r:id="rId15" ref="I16"/>
+    <hyperlink r:id="rId16" ref="I17"/>
+    <hyperlink r:id="rId17" ref="I18"/>
+    <hyperlink r:id="rId18" ref="I19"/>
+    <hyperlink r:id="rId19" ref="I20"/>
+    <hyperlink r:id="rId20" ref="I21"/>
+    <hyperlink r:id="rId21" ref="I22"/>
+    <hyperlink r:id="rId22" ref="I23"/>
+    <hyperlink r:id="rId23" ref="I24"/>
+    <hyperlink r:id="rId24" ref="I25"/>
+    <hyperlink r:id="rId25" ref="I26"/>
+    <hyperlink r:id="rId26" ref="I27"/>
+    <hyperlink r:id="rId27" ref="I28"/>
   </hyperlinks>
-  <drawing r:id="rId6"/>
+  <drawing r:id="rId28"/>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId30"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
base de datos con productos eufar
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="127">
   <si>
     <t>id</t>
   </si>
@@ -108,6 +108,331 @@
     <t>https://res.cloudinary.com/diqmtzief/image/upload/v1731095332/tnW0NfBg_uffal6.png</t>
   </si>
   <si>
+    <t>Detergente Multienzimático Bonzyme</t>
+  </si>
+  <si>
+    <t>Disponible en presentaciones de 90ml, 1 litro, galón y 5 litros.
+El Detergente Multienzimático Bonzyme es una solución concentrada diseñada para la limpieza profunda de instrumentos odontológicos y médicos. Su fórmula contiene múltiples enzimas que descomponen eficazmente residuos orgánicos como sangre, proteínas y tejidos, facilitando la esterilización completa. Es una herramienta esencial para mantener un alto estándar de higiene y prevenir infecciones en entornos clínicos.</t>
+  </si>
+  <si>
+    <t>Fórmula multienzimática que asegura una limpieza profunda.
+Compatible con acero inoxidable, vidrio y otros materiales de instrumental clínico.
+Biodegradable y seguro para el medio ambiente.
+Disponible en diferentes presentaciones para adaptarse a las necesidades del consultorio.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732220634/45oFikcw_rubfc6.png</t>
+  </si>
+  <si>
+    <t>Alvofar Plus Pote x 10 gr</t>
+  </si>
+  <si>
+    <t>El Alvofar Plus es un material terapéutico diseñado para el tratamiento de alveolitis y la protección de cavidades post-extracción dental. Su fórmula avanzada alivia el dolor, controla la inflamación y acelera el proceso de cicatrización. Este producto es ampliamente utilizado en odontología por su eficacia en el manejo de complicaciones postquirúrgicas, proporcionando comodidad y rápida recuperación a los pacientes.</t>
+  </si>
+  <si>
+    <t>Presentación en pote de 10g, ideal para múltiples aplicaciones.
+Formulación especializada para el manejo de alveolitis.
+Efecto analgésico, antiinflamatorio y cicatrizante.
+Fácil aplicación directa en la cavidad post-extracción.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732219502/-iCaqnbA_zeh3wm.png</t>
+  </si>
+  <si>
+    <t>Acido Fluorhídrico 9.6%</t>
+  </si>
+  <si>
+    <t>El Ácido Fluorhídrico 9.6% de Eufar es un agente químico utilizado en odontología para el grabado de porcelanas y cerámicas dentales. Este producto prepara las superficies cerámicas para mejorar la adhesión de resinas compuestas y cementos adhesivos, garantizando un fuerte enlace mecánico entre el material restaurador y la superficie dental. Es un material esencial en procedimientos de odontología estética y restauradora.</t>
+  </si>
+  <si>
+    <t>Concentración del 9.6%, óptima para el grabado de porcelanas y cerámicas dentales.
+Mejora la adhesión de resinas compuestas y cementos adhesivos.
+Presentación segura y práctica para uso clínico.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732219082/S7xT5C1w_fbqhui.jpg</t>
+  </si>
+  <si>
+    <t>Jabon Bonfar Galon</t>
+  </si>
+  <si>
+    <t>El Jabón Bonfar en presentación de galón es un jabón líquido antibacterial de alta calidad, ideal para garantizar la higiene en entornos clínicos y odontológicos. Formulado para eliminar bacterias y gérmenes de manera eficaz, es una solución económica y práctica para el uso frecuente en consultorios y clínicas, promoviendo un ambiente seguro y limpio para pacientes y profesionales.</t>
+  </si>
+  <si>
+    <t>Presentación en galón (4 litros), ideal para uso continuo.
+Fórmula antibacterial que elimina gérmenes y bacterias.
+Suave con la piel, adecuado para el lavado frecuente de manos.
+Recomendado para consultorios odontológicos y entornos médicos.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732220249/EFcn0Irg_xuixjc.png</t>
+  </si>
+  <si>
+    <t>Jabon Bonfar x 500ml</t>
+  </si>
+  <si>
+    <t>El Jabón Bonfar de Eufar es un jabón líquido antibacterial especialmente formulado para garantizar una limpieza eficaz y segura en entornos clínicos. Su fórmula suave protege la piel mientras elimina bacterias y otros agentes patógenos, siendo ideal para el uso en consultorios odontológicos y áreas de atención médica. Este producto es indispensable para mantener altos estándares de higiene y prevenir infecciones cruzadas.</t>
+  </si>
+  <si>
+    <t>Presentación en envase de 500ml con dosificador para fácil aplicación.
+Fórmula antibacterial que elimina eficazmente gérmenes.
+Suave con la piel, apto para uso frecuente.
+Ideal para clínicas odontológicas y ambientes clínicos.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732220036/wLF63Rkw_lxjpw9.png</t>
+  </si>
+  <si>
+    <t>Dentofar x 5ml Desensibilizante</t>
+  </si>
+  <si>
+    <t>El Dentofar es un desensibilizante de alta eficacia diseñado para tratar la hipersensibilidad dental, proporcionando alivio rápido y duradero. Su fórmula especializada actúa bloqueando los túbulos dentinarios expuestos, reduciendo la sensibilidad al contacto con alimentos, bebidas o estímulos térmicos. Es un producto indispensable en tratamientos restaurativos y preventivos en odontología.</t>
+  </si>
+  <si>
+    <t>Presentación en frasco de 5 ml con aplicador preciso.
+Fórmula diseñada para bloquear los túbulos dentinarios.
+Proporciona alivio inmediato y duradero de la sensibilidad dental.
+Seguro y eficaz en dientes naturales y restauraciones.</t>
+  </si>
+  <si>
+    <t>Restaurativos</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732221029/snFk_1jQ_ocmmy1.png</t>
+  </si>
+  <si>
+    <t>Pasta Profilactica Detarfar Colapsible</t>
+  </si>
+  <si>
+    <t>La Pasta Profiláctica Detarfar es un producto diseñado para la limpieza y el pulido dental profesional. Con propiedades desensibilizantes, esta pasta ayuda a eliminar manchas, placa y depósitos suaves, dejando una superficie dental lisa y preparada para procedimientos posteriores. Es ideal para consultas preventivas y restaurativas.</t>
+  </si>
+  <si>
+    <t>Fórmula con propiedades desensibilizantes para mayor confort del paciente.
+Textura y grano adecuados para una limpieza eficaz sin dañar el esmalte.
+Disponible en dos presentaciones prácticas: 50g (ideal para uso específico) y 12 onzas (uso frecuente en consultorio).
+Compatible con el uso de cepillos o copas de profilaxis.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732221518/d-01fPEQ_nixdwe.png</t>
+  </si>
+  <si>
+    <t>Polvo Detarfar Prophy 120g</t>
+  </si>
+  <si>
+    <t>El Polvo Detarfar Prophy es un producto de alta calidad diseñado para procedimientos de profilaxis dental profesional. Este polvo es ideal para la limpieza profunda de manchas, placa y depósitos dentales en combinación con equipos de limpieza por aire. Su fórmula es suave con el esmalte, dejando una superficie dental perfectamente pulida y preparada para otros tratamientos.</t>
+  </si>
+  <si>
+    <t>Presentación de 120g, ideal para uso profesional en consultorios.
+Fórmula efectiva y segura para la eliminación de manchas y placa.
+Compatible con equipos de limpieza por aire y sistemas de abrasión dental.
+Textura diseñada para no dañar el esmalte ni causar molestias al paciente.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732221711/v0u25_LQ_wxrvx2.png</t>
+  </si>
+  <si>
+    <t>Revelador de Placa Ditono x 10ml</t>
+  </si>
+  <si>
+    <t>El Revelador de Placa Ditono es un producto diseñado para resaltar la presencia de placa bacteriana en los dientes, facilitando su identificación durante las consultas odontológicas o en el cuidado bucal personal. Su fórmula coloreada permite identificar áreas con mala higiene o acumulación de placa, ayudando a mejorar la técnica de cepillado y prevenir problemas dentales.</t>
+  </si>
+  <si>
+    <t>Presentación en frasco de 10ml, práctico y fácil de usar.
+Fórmula segura y efectiva que resalta la placa bacteriana con un color distintivo.
+Ideal para uso profesional en consultorios y también para la educación en higiene bucal en casa.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732221948/ycsb98wA_j7m6bm.png</t>
+  </si>
+  <si>
+    <t>Eucida Advanced x 750ml</t>
+  </si>
+  <si>
+    <t>Eucida Advanced es un desinfectante y limpiador de alta eficacia diseñado para el entorno odontológico. Su fórmula avanzada permite una limpieza profunda y desinfección de superficies, equipos e instrumentos dentales, eliminando microorganismos patógenos y garantizando un entorno clínico seguro. Ideal para la limpieza de consultorios odontológicos y de superficies que entran en contacto con pacientes.</t>
+  </si>
+  <si>
+    <t>Presentación de 750ml, ideal para uso frecuente en consultorios odontológicos.
+Eficaz contra una amplia gama de bacterias, virus y hongos.
+Producto listo para usar, sin necesidad de dilución.
+Apto para superficies duras, equipos, muebles y utensilios en consultorios dentales.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732222265/17bnYlMQ_t9ilka.png</t>
+  </si>
+  <si>
+    <t>Eugenol Eufar x 15ml</t>
+  </si>
+  <si>
+    <t>El Eugenol Eufar es un producto odontológico utilizado por su capacidad anestésica, antiinflamatoria y como material base en procedimientos restaurativos. Se emplea comúnmente en el tratamiento de dientes temporales, obturaciones provisionales y como auxiliar en el manejo de la pulpa dental. Gracias a su acción calmante y su alta efectividad, es esencial en la odontología para ofrecer comodidad al paciente durante los procedimientos.</t>
+  </si>
+  <si>
+    <t>Presentación de 15ml, adecuado para uso profesional.
+Propiedades analgésicas, lo que ayuda a reducir el dolor y la incomodidad durante tratamientos temporales.
+Ideal para mezclarse con otros materiales como óxido de zinc para crear cementos temporales o bases protectoras.
+También utilizado en la preparación de medicamentos y pastas utilizadas para la desinfección de conductos radiculares.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732222515/mW3gz_tA_gvc5iu.png</t>
+  </si>
+  <si>
+    <t>Gel Antibacterial Farben 65% x 500ml</t>
+  </si>
+  <si>
+    <t>El Gel Antibacterial Farben con un 65% de concentración de alcohol es ideal para la desinfección rápida y eficaz de las manos en entornos odontológicos y clínicos. Su formulación avanzada permite una limpieza profunda, eliminando hasta el 99.9% de los gérmenes y bacterias, sin necesidad de agua. Este gel es un indispensable en la práctica diaria de la odontología, tanto para el personal de la clínica como para los pacientes, ayudando a mantener estándares de higiene rigurosos.</t>
+  </si>
+  <si>
+    <t>Concentración de 65% de alcohol, garantizando una acción antimicrobiana efectiva.
+Presentación de 500ml, ideal para uso continuo en clínicas y consultorios odontológicos.
+Textura de gel, fácil de aplicar y de rápida absorción sin dejar residuos pegajosos.
+Higieniza y desinfecta las manos eliminando hasta el 99.9% de bacterias y virus.
+No requiere enjuague con agua, lo que permite una desinfección rápida en cualquier momento.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732222732/UaoolzRg_dniiwt.png</t>
+  </si>
+  <si>
+    <t>Fluofar Chicle</t>
+  </si>
+  <si>
+    <t>El Fluofar Chicle es un gel fluorado diseñado para la aplicación tópica en pacientes, proporcionando una protección efectiva contra las caries. Con su agradable sabor a chicle, este producto se utiliza principalmente en procedimientos odontológicos preventivos, permitiendo la remineralización del esmalte dental y la prevención de la aparición de caries.</t>
+  </si>
+  <si>
+    <t>Presentación en 240ml y 500ml, ideal para su uso en consultorios y clínicas odontológicas.
+Sabor agradable a chicle, lo que lo hace más atractivo y cómodo para los pacientes, especialmente los niños.
+Fórmula fluorinada, rica en flúor para proporcionar una protección efectiva contra las caries y fortalecer el esmalte dental.
+Producto de uso profesional: se utiliza en tratamientos de prevención y protección dental, aplicable de forma rápida y fácil en las consultas.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732222972/uRuxE_jQ_ifcfcp.png</t>
+  </si>
+  <si>
+    <t>Glutfar 2% Galon</t>
+  </si>
+  <si>
+    <t>El Glutfar 2% es un desinfectante de amplio espectro, especialmente formulado para la desinfección de superficies, equipos e instrumentos en clínicas odontológicas. Su concentración al 2% de glutaraldehído lo convierte en un potente germicida, bactericida, virucida y fungicida, ideal para la limpieza profunda en consultorios odontológicos, hospitales y clínicas.</t>
+  </si>
+  <si>
+    <t>Concentración al 2% de glutaraldehído, un potente desinfectante de amplio espectro.
+Presentación de 1 galón (3.78 L), adecuado para el uso continuo en clínicas y consultorios odontológicos.
+Eficaz contra una amplia gama de patógenos, incluyendo virus, bacterias y hongos.
+Etiqueta verde, lo que indica que está formulado para su uso en áreas clínicas y de atención a pacientes.
+Fórmula de acción rápida, ideal para la desinfección de superficies y equipos no invasivos.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732223204/uHi3SYzg_kxdo6w.png</t>
+  </si>
+  <si>
+    <t>Tirillas De Verificacion x 100 und Quantofix</t>
+  </si>
+  <si>
+    <t>Las Tirillas de Verificación Quantofix son herramientas precisas y confiables para la medición rápida de diversos parámetros en el entorno odontológico, como la presencia de compuestos o el nivel de pH. Este producto es indispensable para profesionales que necesitan realizar verificaciones rápidas y efectivas durante sus procedimientos.</t>
+  </si>
+  <si>
+    <t>Presentación de 100 tirillas, garantizando un uso prolongado y económico en clínicas odontológicas.
+Alta precisión en la medición de sustancias, proporcionando resultados rápidos y fiables.
+Fácil uso: ideal para ser empleada en cualquier procedimiento donde se necesite controlar la calidad de los compuestos utilizados o verificar la concentración de ciertos materiales.
+Versátil: adecuado para medir una amplia variedad de sustancias utilizadas en odontología.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732223412/g56X37mA_xaepyw.png</t>
+  </si>
+  <si>
+    <t>Glutfar 2% Plus HLD</t>
+  </si>
+  <si>
+    <t>El Glutfar 2% Plus HLD es una solución desinfectante de alta eficacia diseñada para la desinfección de instrumentos odontológicos y equipos médicos no invasivos. Su potente formulación con un 2% de glutaraldehído asegura una acción antimicrobiana efectiva contra bacterias, virus, hongos y esporas, lo que lo convierte en un producto indispensable para la esterilización de material odontológico en clínicas y consultorios.</t>
+  </si>
+  <si>
+    <t>Concentración de 2% de glutaraldehído: potente y eficaz contra microorganismos patógenos.
+Presentación en 5 litros, 1 litro, 500ml y galón: ideal para uso clínico con diferentes necesidades de volumen.
+Desinfección de alto nivel (HLD): asegura la eliminación de microorganismos y esporas, proporcionando seguridad en la manipulación de los instrumentos.
+Apto para la desinfección de instrumentos dentales de metal, plástico y otros materiales comunes en la práctica odontológica.
+Fórmula de acción rápida que no deja residuos tóxicos en los instrumentos.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732223741/WEM7yGdw_gdix3c.png</t>
+  </si>
+  <si>
+    <t>Cemento Grossfar 10gr</t>
+  </si>
+  <si>
+    <t>El Cemento Grossfar 10gr Eufar es un material dental de alta calidad, especialmente formulado para la fijación de restauraciones dentales como coronas, puentes, carillas y otros elementos protésicos. Su característica principal es su capacidad de adherir con firmeza y durabilidad, proporcionando un ajuste preciso y seguro.</t>
+  </si>
+  <si>
+    <t>Presentación de 10gr, ideal para varios procedimientos de fijación dental.
+Fijación fuerte y duradera: asegura una adherencia efectiva, garantizando que las restauraciones permanezcan en su lugar durante un largo período de tiempo.
+Fácil de mezclar y aplicar, lo que facilita su uso en el consultorio dental y reduce los tiempos de procedimiento.
+Resistencia al desgaste y a las cargas masticatorias, proporcionando estabilidad a largo plazo.
+Compatible con otros materiales restaurativos y adhesivos dentales.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732223939/UXMvj6pg_z8yx39.png</t>
+  </si>
+  <si>
+    <t>Hemofar x 7ml</t>
+  </si>
+  <si>
+    <t>Hemofar es un hemostático de uso odontológico, especialmente formulado para el control y manejo de hemorragias durante procedimientos dentales. Presentado en un envase de 7ml, este producto ayuda a detener rápidamente el sangrado, facilitando la realización de tratamientos sin complicaciones por sangrado excesivo.</t>
+  </si>
+  <si>
+    <t>Presentación de 7ml, ideal para ser utilizado en diversos procedimientos dentales.
+Fórmula hemostática, que actúa rápidamente sobre la zona afectada para controlar las hemorragias.
+Fácil aplicación, generalmente utilizado en áreas orales donde se presenta sangrado durante o después de un tratamiento.
+Producto estéril, garantizando la seguridad del paciente durante su uso.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732224144/l5a6I_rQ_k7rq4x.png</t>
+  </si>
+  <si>
+    <t>Momifar x 7ml</t>
+  </si>
+  <si>
+    <t>El Momifar Eufar es un desensibilizante dental de alta eficacia, formulado para aliviar la sensibilidad dental en pacientes que experimentan dolor o incomodidad debido a la exposición de las terminaciones nerviosas en los dientes. Este producto es especialmente útil durante y después de tratamientos de restauración o limpieza profunda, proporcionando un alivio inmediato y prolongado.</t>
+  </si>
+  <si>
+    <t>Presentación de 7ml, ideal para tratamientos puntuales en consultorios odontológicos.
+Eficaz contra la sensibilidad dental en pacientes, proporcionando alivio rápido tras procedimientos.
+Fórmula de fácil aplicación que actúa en pocos minutos.
+Apto para su uso en pacientes con dientes sensibles o que requieren tratamientos invasivos.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732224457/tmyjgnrg_uqgzfe.png</t>
+  </si>
+  <si>
+    <t>Oxido de Zinc x 175g</t>
+  </si>
+  <si>
+    <t>El Óxido de Zinc Eufar es un polvo de alta calidad utilizado en odontología para la preparación de cementos dentales y como componente en la fabricación de otros materiales restauradores. Es un producto esencial en la creación de mezclas para el tratamiento de cavidades y la fabricación de selladores temporales. Su alta pureza y propiedades biocompatibles lo hacen ideal para una variedad de procedimientos odontológicos.</t>
+  </si>
+  <si>
+    <t>Presentación de 175g, una cantidad ideal para su uso en clínicas odontológicas.
+Alta pureza y calidad, asegurando la efectividad en los tratamientos.
+Utilizado en la preparación de cementos dentales, material base para restauraciones y recubrimientos.
+Excelente biocompatibilidad, minimizando el riesgo de reacciones adversas en los pacientes.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732224556/MWIyIXoQ_fsq83c.png</t>
+  </si>
+  <si>
+    <t>Perifar Restaurador de Autoclave x 750ml</t>
+  </si>
+  <si>
+    <t>El Perifar Restaurador de Autoclave es una solución especializada para la limpieza, mantenimiento y restauración de equipos de esterilización, como autoclaves. Este producto es ideal para remover residuos de minerales, óxido y otras impurezas que puedan acumularse con el tiempo, prolongando la vida útil del equipo y asegurando su correcto funcionamiento.</t>
+  </si>
+  <si>
+    <t>Fórmula efectiva diseñada para limpiar y restaurar superficies internas y externas de autoclaves.
+Capacidad de 750ml, ideal para uso frecuente en clínicas y consultorios odontológicos.
+Ayuda a prevenir la acumulación de residuos de cal y minerales.
+Contribuye al mantenimiento del equipo, mejorando su rendimiento y extendiendo su vida útil.
+Producto seguro para equipos de acero inoxidable y otros materiales comunes en autoclaves.</t>
+  </si>
+  <si>
+    <t>Equipos</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732309213/Perifar_autoclave_Alta__3_-removebg-preview_jp3lxe.png</t>
+  </si>
+  <si>
     <t>Adhesivo Prime &amp; Bond Universal</t>
   </si>
   <si>
@@ -120,20 +445,45 @@
 Presentación fácil de usar que optimiza los tiempos de aplicación</t>
   </si>
   <si>
-    <t>Accesorios</t>
-  </si>
-  <si>
     <t>Dentsply Sirona</t>
   </si>
   <si>
     <t>https://res.cloudinary.com/diqmtzief/image/upload/v1731614688/primebond-universal_o1cfsi.jpg</t>
+  </si>
+  <si>
+    <t>Resina Spectra Basic A2 Jeringa 4g</t>
+  </si>
+  <si>
+    <t>La Resina Spectra Basic A2 de Dentsply Sirona es un material de restauración dental de alta calidad diseñado para la reconstrucción estética y funcional de dientes anteriores y posteriores. Su fórmula avanzada garantiza una excelente manipulación, fácil modelado, y un acabado de alta estética, ideal para procedimientos restauradores directos. Con un tono universal A2, se adapta fácilmente al color natural del diente, asegurando resultados duraderos y estéticamente agradables.</t>
+  </si>
+  <si>
+    <t>Presentación en jeringa de 4g para aplicaciones directas y precisas.
+Tono A2 universal que se adapta a múltiples tonalidades dentales.
+Excelente resistencia mecánica y acabado brillante.
+Ideal para restauraciones en dientes anteriores y posteriores.
+Fácil de manipular, con propiedades de baja contracción.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732218579/resina-spectra-basic-jeringa.jpg_umh4ld.png</t>
+  </si>
+  <si>
+    <t>producto prubea</t>
+  </si>
+  <si>
+    <t>prueba</t>
+  </si>
+  <si>
+    <t>Ortodoncia</t>
+  </si>
+  <si>
+    <t>Densell</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -156,6 +506,21 @@
       <name val="Roboto"/>
     </font>
     <font>
+      <color rgb="FF434343"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
       <color rgb="FF434343"/>
       <name val="Roboto"/>
     </font>
@@ -353,7 +718,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -405,17 +770,20 @@
     <xf borderId="6" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="9" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -478,7 +846,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I7" displayName="Productos" name="Productos" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I29" displayName="Productos" name="Productos" id="1">
   <tableColumns count="9">
     <tableColumn name="id" id="1"/>
     <tableColumn name="nombre" id="2"/>
@@ -853,39 +1221,639 @@
       <c r="A6" s="5">
         <v>5.0</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="14" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="14" t="s">
+    </row>
+    <row r="7">
+      <c r="A7" s="9">
+        <v>6.0</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="16" t="s">
+      <c r="C7" s="11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="17"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="21"/>
+      <c r="D7" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="7"/>
+      <c r="I8" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="9">
+        <v>8.0</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="5">
+        <v>9.0</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="9">
+        <v>10.0</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="12"/>
+      <c r="I11" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="5">
+        <v>11.0</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="7"/>
+      <c r="I12" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="9">
+        <v>12.0</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="5">
+        <v>13.0</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="9">
+        <v>14.0</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="12"/>
+      <c r="I15" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="5">
+        <v>15.0</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="9">
+        <v>16.0</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="5">
+        <v>17.0</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="7"/>
+      <c r="I18" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="9">
+        <v>18.0</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="12"/>
+      <c r="I19" s="17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="5">
+        <v>19.0</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="I20" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="9">
+        <v>20.0</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="12"/>
+      <c r="I21" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="5">
+        <v>21.0</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="I22" s="16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="9">
+        <v>22.0</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="12"/>
+      <c r="I23" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="5">
+        <v>23.0</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="7"/>
+      <c r="I24" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="9">
+        <v>24.0</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H25" s="12"/>
+      <c r="I25" s="18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="5">
+        <v>25.0</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" s="19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="9">
+        <v>26.0</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="12"/>
+      <c r="I27" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="5">
+        <v>27.0</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="7"/>
+      <c r="I28" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="20">
+        <v>28.0</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="F29" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="G29" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29" s="22">
+        <v>5.0</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -894,10 +1862,32 @@
     <hyperlink r:id="rId3" ref="I4"/>
     <hyperlink r:id="rId4" ref="I5"/>
     <hyperlink r:id="rId5" ref="I6"/>
+    <hyperlink r:id="rId6" ref="I7"/>
+    <hyperlink r:id="rId7" ref="I8"/>
+    <hyperlink r:id="rId8" ref="I9"/>
+    <hyperlink r:id="rId9" ref="I10"/>
+    <hyperlink r:id="rId10" ref="I11"/>
+    <hyperlink r:id="rId11" ref="I12"/>
+    <hyperlink r:id="rId12" ref="I13"/>
+    <hyperlink r:id="rId13" ref="I14"/>
+    <hyperlink r:id="rId14" ref="I15"/>
+    <hyperlink r:id="rId15" ref="I16"/>
+    <hyperlink r:id="rId16" ref="I17"/>
+    <hyperlink r:id="rId17" ref="I18"/>
+    <hyperlink r:id="rId18" ref="I19"/>
+    <hyperlink r:id="rId19" ref="I20"/>
+    <hyperlink r:id="rId20" ref="I21"/>
+    <hyperlink r:id="rId21" ref="I22"/>
+    <hyperlink r:id="rId22" ref="I23"/>
+    <hyperlink r:id="rId23" ref="I24"/>
+    <hyperlink r:id="rId24" ref="I25"/>
+    <hyperlink r:id="rId25" ref="I26"/>
+    <hyperlink r:id="rId26" ref="I27"/>
+    <hyperlink r:id="rId27" ref="I28"/>
   </hyperlinks>
-  <drawing r:id="rId6"/>
+  <drawing r:id="rId28"/>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId30"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
base de datos con productos eufar 3
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="123">
   <si>
     <t>id</t>
   </si>
@@ -465,18 +465,6 @@
   </si>
   <si>
     <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732218579/resina-spectra-basic-jeringa.jpg_umh4ld.png</t>
-  </si>
-  <si>
-    <t>producto prubea</t>
-  </si>
-  <si>
-    <t>prueba</t>
-  </si>
-  <si>
-    <t>Ortodoncia</t>
-  </si>
-  <si>
-    <t>Densell</t>
   </si>
 </sst>
 </file>
@@ -544,7 +532,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="10">
     <border/>
     <border>
       <left style="thin">
@@ -672,53 +660,11 @@
         <color rgb="FFF6F8F9"/>
       </bottom>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF284E3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFF6F8F9"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFF6F8F9"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF284E3F"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFF6F8F9"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFF6F8F9"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFF6F8F9"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF284E3F"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFF6F8F9"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF284E3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFF6F8F9"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF284E3F"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -777,15 +723,6 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -1829,32 +1766,6 @@
         <v>122</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="20">
-        <v>28.0</v>
-      </c>
-      <c r="B29" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="C29" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="D29" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="E29" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="F29" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="G29" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="I29" s="22">
-        <v>5.0</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="I2"/>

</xml_diff>

<commit_message>
Base de datos, proquident
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -5,13 +5,15 @@
   <sheets>
     <sheet state="visible" name="Productos" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Productos!$A$1:$I$73</definedName>
+  </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="296">
   <si>
     <t>id</t>
   </si>
@@ -427,9 +429,6 @@
 Producto seguro para equipos de acero inoxidable y otros materiales comunes en autoclaves.</t>
   </si>
   <si>
-    <t>Equipos</t>
-  </si>
-  <si>
     <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732309213/Perifar_autoclave_Alta__3_-removebg-preview_jp3lxe.png</t>
   </si>
   <si>
@@ -466,12 +465,870 @@
   <si>
     <t>https://res.cloudinary.com/diqmtzief/image/upload/v1732218579/resina-spectra-basic-jeringa.jpg_umh4ld.png</t>
   </si>
+  <si>
+    <t>Resina Surefil SDR Kit</t>
+  </si>
+  <si>
+    <t>La Resina Surefil SDR es un innovador material de restauración dental diseñado para aplicaciones en restauraciones posteriores como base o liner. Su tecnología avanzada facilita el manejo, mejora la adaptación a la cavidad y reduce el estrés de contracción, proporcionando una solución eficiente y confiable para los profesionales odontológicos.</t>
+  </si>
+  <si>
+    <t>Tecnología SDR (Smart Dentin Replacement): Permite colocaciones en incrementos de hasta 4 mm, ahorrando tiempo en comparación con resinas convencionales.
+Fluidez óptima: Su consistencia autoadaptable asegura una cobertura uniforme y completa de las cavidades.
+Baja contracción: Reduce el estrés de contracción, minimizando las posibilidades de sensibilidad postoperatoria y asegurando una restauración duradera.
+Estética mejorada: Compatible con resinas compuestas universales para una capa final altamente estética.
+Radiopacidad alta: Facilita su identificación en radiografías, asegurando un diagnóstico preciso.
+Kit completo con jeringa y puntas aplicadoras para mayor precisión y facilidad de uso.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1733504853/resina-surefilSDR_kit_kqxvpy.png</t>
+    </r>
+  </si>
+  <si>
+    <t>AH Plus®</t>
+  </si>
+  <si>
+    <t>AH Plus® es un sellador de conductos radiculares de dos componentes (base y catalizador) diseñado para procedimientos de endodoncia. Su formulación avanzada a base de resina epoxi asegura un sellado hermético, duradero y biocompatible, minimizando el riesgo de filtración y reinfección en el tratamiento de conductos.</t>
+  </si>
+  <si>
+    <t>Alta capacidad de sellado: Su baja contracción y excelente fluidez permiten una perfecta adaptación a las paredes del conducto.
+Biocompatible: Minimiza la irritación tisular, lo que lo hace seguro para los pacientes.
+Radiopaco: Facilita su visualización en radiografías para un diagnóstico y control precisos.
+Tiempo de trabajo adecuado: Ofrece un tiempo suficiente para su manipulación y colocación antes del fraguado.
+Fácil mezcla y aplicación: Su presentación en pasta-pasta permite una preparación rápida y uniforme.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734442604/Imagen_de_WhatsApp_2024-12-16_a_las_08.31.15_047d5b66_fae1ro.jpg</t>
+    </r>
+  </si>
+  <si>
+    <t>Forro Dentinario Dycal Fórmula Avanzada II</t>
+  </si>
+  <si>
+    <t>Dycal Fórmula Avanzada II es un forrador dentinario a base de hidróxido de calcio radiopaco. Se utiliza en procedimientos odontológicos para proteger la pulpa dental y promover la formación de dentina secundaria. Es ideal para utilizar como base en restauraciones profundas, ya que actúa como aislante térmico y eléctrico.</t>
+  </si>
+  <si>
+    <t>Base de hidróxido de calcio radiopaco: Ayuda a la protección de la pulpa dental en cavidades profundas.
+Estimula la formación de dentina secundaria: Promueve la reparación natural del diente y protege contra lesiones adicionales.
+Radiopacidad alta: Facilita su identificación en radiografías para un control clínico adecuado.
+Fácil manipulación: Viene en una fórmula de dos componentes (base y catalizador) que se mezclan fácilmente para una aplicación uniforme.
+Aislante térmico y eléctrico: Protege la pulpa dental de estímulos térmicos o eléctricos provenientes de restauraciones.
+Rápida colocación y endurecimiento: Mejora la eficiencia en procedimientos clínicos.
+Baja solubilidad: Garantiza durabilidad y estabilidad en el tiempo.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734443126/Imagen_de_WhatsApp_2024-12-16_a_las_08.31.03_e91130bc_bsmtja.jpg</t>
+  </si>
+  <si>
+    <t>Cavitron® Prophy Powder</t>
+  </si>
+  <si>
+    <t>El Cavitron® Prophy Powder es un polvo profiláctico de bicarbonato de sodio con sabor a menta, especialmente diseñado para la limpieza profesional de los dientes mediante dispositivos de ultrasonido. Su fórmula proporciona una acción efectiva y cómoda para el paciente, eliminando la placa y manchas superficiales con rapidez.</t>
+  </si>
+  <si>
+    <t>Eliminación eficaz de manchas y placa: Actúa de manera eficiente para eliminar biofilm, manchas y depósitos superficiales en los dientes.
+Sabor refrescante a menta: Ofrece una experiencia más agradable para el paciente durante el procedimiento profiláctico.
+Uso con equipos de ultrasonido: Compatible con dispositivos Cavitron® y sistemas de profilaxis por aire, permitiendo un tratamiento rápido y efectivo.
+Fina granulometría: Asegura una aplicación controlada y suave, minimizando la abrasión en la superficie dental.
+Presentación práctica: Envase hermético de 13 oz (364 g) para mantener la frescura y calidad del polvo.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734444816/DSCF3291-removebg-preview-a64J5Y63l-transformed-removebg-preview_sfnpuf.png</t>
+    </r>
+  </si>
+  <si>
+    <t>Agua Desionizada 3800 ml</t>
+  </si>
+  <si>
+    <t>El Agua Desionizada es un producto de alta pureza, libre de minerales y contaminantes, diseñado para ser utilizado en diversos procedimientos odontológicos y médicos. Su fórmula desionizada garantiza la máxima seguridad y eficiencia en procesos que requieren agua de alta calidad, protegiendo equipos y mejorando los resultados clínicos.</t>
+  </si>
+  <si>
+    <t>Alta pureza: Libre de minerales, metales pesados y contaminantes, ideal para usos profesionales.
+Uso versátil: Recomendado para la preparación de soluciones, autoclaves, limpieza de instrumentos y equipos odontológicos.
+Protección de equipos: Minimiza el riesgo de acumulación de depósitos minerales en dispositivos como autoclaves y sistemas de irrigación.
+Presentación práctica: Envase de 3800 ml que asegura un suministro adecuado para diferentes necesidades clínicas.
+Compatible con normas sanitarias: Cumple con los estándares requeridos para uso odontológico y médico.</t>
+  </si>
+  <si>
+    <t>Proquident</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734705160/AGUA_DESIONIZADA_be3zbo.png</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Cepillo Interproximal </t>
+  </si>
+  <si>
+    <t>El Cepillo Interproximal es una herramienta esencial para la higiene bucal diaria, diseñada específicamente para la limpieza efectiva de los espacios interdentales y alrededor de aparatos de ortodoncia. Su diseño cilíndrico permite acceder a áreas difíciles de alcanzar con un cepillo dental convencional, eliminando la placa bacteriana y promoviendo una salud bucal óptima.</t>
+  </si>
+  <si>
+    <t>Diseño cilíndrico y flexible: Facilita la limpieza profunda de espacios interdentales, incluso en zonas estrechas o de difícil acceso.
+Remoción efectiva de placa: Ayuda a prevenir caries, gingivitis y acumulación de bacterias en los espacios interdentales y alrededor de brackets o retenedores.
+Mango ergonómico: Proporciona un agarre cómodo y seguro para un uso sencillo y preciso.
+Uso seguro y versátil: Ideal para pacientes con ortodoncia, implantes, coronas o prótesis dentales.
+Presentación práctica: Incluye 4 unidades individuales, perfectas para uso personal o clínico.</t>
+  </si>
+  <si>
+    <t>Ortodoncia</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734705671/CEPILLO_INTERPROXIMAL_drjngp.png</t>
+    </r>
+  </si>
+  <si>
+    <t>Cepillo Dental para Ortodoncia</t>
+  </si>
+  <si>
+    <t>El Cepillo Dental para Ortodoncia Proquident es una herramienta diseñada especialmente para pacientes en tratamiento de ortodoncia. Gracias a su diseño especializado, permite una limpieza eficaz alrededor de brackets, alambres y otros componentes del tratamiento ortodóntico, garantizando una higiene bucal completa y efectiva.
+Este cepillo combina tecnología y comodidad para proteger la salud bucal durante el uso de aparatos ortodónticos, ayudando a prevenir problemas como caries, gingivitis o acumulación de placa bacteriana.</t>
+  </si>
+  <si>
+    <t>Cerdas en forma de "V": Diseñadas específicamente para limpiar alrededor de los brackets y alambres, facilitando el acceso a zonas difíciles.
+Mango ergonómico: Ofrece un agarre cómodo y seguro para un mejor control durante el cepillado.
+Cabezal compacto: Ideal para alcanzar áreas de difícil acceso, garantizando una limpieza profunda.
+Material de alta calidad: Fabricado con materiales duraderos y seguros, recomendados por odontólogos.
+Uso diario: Diseñado para usarse de manera cotidiana como complemento del cepillado convencional.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734706179/CEPILLO_ORTODONCIA_jzclgb.jpg</t>
+    </r>
+  </si>
+  <si>
+    <t>Crema Carbon X 25 g</t>
+  </si>
+  <si>
+    <t>La Crema Carbon X 25 g es un producto especializado que combina las propiedades del carbón activado con agentes limpiadores avanzados para proporcionar una limpieza profunda y efectiva. Diseñada para remover manchas, eliminar la placa bacteriana y mantener un aliento fresco, esta crema es ideal para quienes buscan un cuidado bucal superior.
+Es una excelente opción para procedimientos restaurativos, ya que ayuda a mantener la limpieza y el brillo de restauraciones dentales, previniendo la acumulación de manchas o decoloraciones.</t>
+  </si>
+  <si>
+    <t>Carbón activado: Ingrediente natural que contribuye a la eliminación de manchas y el control de toxinas.
+Textura suave: Diseñada para ser delicada con las restauraciones dentales y los tejidos bucales.
+Efecto blanqueador: Ayuda a recuperar y mantener el color natural de los dientes sin dañar el esmalte.
+Frescura duradera: Proporciona un aliento fresco gracias a su fórmula avanzada.
+Fácil aplicación: Presentación en tubo compacto de 25 g, ideal para uso diario y fácil de transportar.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734706444/CREMA_CARBON_25G_lishbf.png</t>
+    </r>
+  </si>
+  <si>
+    <t>Crema Carbon X 75 g</t>
+  </si>
+  <si>
+    <t>La Crema Carbon X 75 g es un producto especializado que combina las propiedades del carbón activado con agentes limpiadores avanzados para proporcionar una limpieza profunda y efectiva. Diseñada para remover manchas, eliminar la placa bacteriana y mantener un aliento fresco, esta crema es ideal para quienes buscan un cuidado bucal superior.
+Es una excelente opción para procedimientos restaurativos, ya que ayuda a mantener la limpieza y el brillo de restauraciones dentales, previniendo la acumulación de manchas o decoloraciones.</t>
+  </si>
+  <si>
+    <t>Carbón activado: Ingrediente natural que contribuye a la eliminación de manchas y el control de toxinas.
+Textura suave: Diseñada para ser delicada con las restauraciones dentales y los tejidos bucales.
+Efecto blanqueador: Ayuda a recuperar y mantener el color natural de los dientes sin dañar el esmalte.
+Frescura duradera: Proporciona un aliento fresco gracias a su fórmula avanzada.
+Fácil aplicación: Presentación en tubo compacto de 75 g, ideal para uso diario y fácil de transportar.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734707014/CREMA_CARBON_75G_ne5gcb.png</t>
+  </si>
+  <si>
+    <t>Crema Sensitive X 25 g</t>
+  </si>
+  <si>
+    <t>La Crema Sensitive está especialmente formulada para brindar alivio a dientes sensibles, protegiendo el esmalte dental y proporcionando una sensación de frescura y limpieza profunda. Ideal para quienes buscan una solución efectiva y suave para combatir la sensibilidad dental.</t>
+  </si>
+  <si>
+    <t>Alivio para dientes sensibles: Reduce la sensibilidad causada por cambios térmicos, consumo de alimentos fríos o calientes, y desgaste del esmalte.
+Fórmula suave: Contiene ingredientes diseñados para proteger las zonas expuestas y evitar molestias al cepillarse.
+Cuidado restaurador: Fortalece el esmalte y ayuda a prevenir la erosión dental.
+Frescura y limpieza: Deja una sensación agradable de frescura tras su uso.
+Uso recomendado: Apta para el cuidado diario de dientes con sensibilidad, especialmente después de tratamientos odontológicos.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734707231/CREMA_SENSITIVE_25G_ufuvsv.png</t>
+  </si>
+  <si>
+    <t>Crema Sensitive X 75 g</t>
+  </si>
+  <si>
+    <t>La Crema Sensitive de Proquident está especialmente formulada para brindar alivio a dientes sensibles, protegiendo el esmalte dental y proporcionando una sensación de frescura y limpieza profunda. Ideal para quienes buscan una solución efectiva y suave para combatir la sensibilidad dental.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734707230/CREMA_SENSITIVE_75G_eyknse.png</t>
+  </si>
+  <si>
+    <t>Dentafluor Fresa 500g</t>
+  </si>
+  <si>
+    <t>Dentafluor Fresa 500g Proquident es un gel fluorado con un delicioso sabor a fresa, especialmente formulado para proteger el esmalte dental y prevenir la formación de caries. Su presentación en formato de 500g es ideal para uso en consultorios odontológicos, asegurando una aplicación efectiva y profesional.
+Este producto es recomendado para tratamientos de fortalecimiento dental y prevención de caries, siendo una excelente opción tanto para adultos como para niños.</t>
+  </si>
+  <si>
+    <t>Alta concentración de flúor: Refuerza el esmalte dental, haciéndolo más resistente a los ácidos.
+Fórmula neutra: Ideal para dientes sensibles y pacientes que requieren un producto suave y efectivo.
+Prevención de caries: Reduce la incidencia de caries con un uso regular.
+Uso profesional y doméstico: Puede ser utilizado en tratamientos odontológicos o como complemento en el hogar.
+Seguro y de alta calidad: Cumple con los estándares odontológicos para garantizar su efectividad.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734708393/DENTAFLUOR_FRESA_500_rvab9i.png</t>
+  </si>
+  <si>
+    <t>Dentafluor Neutro 500g</t>
+  </si>
+  <si>
+    <t>Dentafluor Neutro 500g es un gel fluorado diseñado para fortalecer el esmalte dental y prevenir la formación de caries. Su fórmula neutra lo hace ideal para pacientes con dientes sensibles o que buscan un producto seguro y efectivo para el cuidado diario de su salud oral.
+Recomendado para complementar tratamientos odontológicos como blanqueamientos, restauraciones o terapias de flúor profesional, garantizando dientes más fuertes y saludables.</t>
+  </si>
+  <si>
+    <t>Alta concentración de flúor: Refuerza el esmalte dental, mejorando su resistencia contra los ácidos y bacterias.
+Sabor agradable a fresa: Facilita su uso, especialmente en pacientes pediátricos.
+Textura de gel: Permite una aplicación uniforme y controlada.
+Uso profesional: Ideal para clínicas y consultorios odontológicos en tratamientos preventivos y de mantenimiento.
+Presentación económica: Su envase de 500g asegura una mayor duración, siendo una opción práctica y eficiente.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734708747/DENTAFLUOR_NEUTRO_500_ssdlwu.png</t>
+  </si>
+  <si>
+    <t>Dentafluor Neutro 50g</t>
+  </si>
+  <si>
+    <t>Dentafluor Neutro 50g es un gel fluorado diseñado para fortalecer el esmalte dental y prevenir la formación de caries. Su fórmula neutra lo hace ideal para pacientes con dientes sensibles o que buscan un producto seguro y efectivo para el cuidado diario de su salud oral.
+Recomendado para complementar tratamientos odontológicos como blanqueamientos, restauraciones o terapias de flúor profesional, garantizando dientes más fuertes y saludables.</t>
+  </si>
+  <si>
+    <t>Alta concentración de flúor: Refuerza el esmalte dental, mejorando su resistencia contra los ácidos y bacterias.
+Sabor agradable a fresa: Facilita su uso, especialmente en pacientes pediátricos.
+Textura de gel: Permite una aplicación uniforme y controlada.
+Uso profesional: Ideal para clínicas y consultorios odontológicos en tratamientos preventivos y de mantenimiento.
+Presentación económica: Su envase de 50g es una opción práctica y eficiente.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734709026/DENTAFLUOR_bitsgp.png</t>
+  </si>
+  <si>
+    <t>Polvo Desmanchador 175g</t>
+  </si>
+  <si>
+    <t>El Polvo Desmanchador 175g es un producto especializado para eliminar manchas y decoloraciones superficiales de los dientes causadas por alimentos, bebidas, tabaco y otros factores. Su fórmula eficaz y segura proporciona una limpieza profunda, ayudando a restaurar el brillo y la blancura natural de los dientes.
+Este producto es ideal para pacientes que desean mejorar la apariencia de su sonrisa de forma profesional y efectiva.</t>
+  </si>
+  <si>
+    <t>Eliminación de manchas superficiales: Actúa eficazmente contra manchas provocadas por café, té, tabaco, vino, entre otros.
+Fórmula segura: Diseñada para proteger el esmalte dental durante su uso.
+Uso profesional o en casa: Puede ser utilizado en consultorios odontológicos o como complemento del cuidado dental diario, según las recomendaciones del odontólogo.
+Fácil aplicación: Se puede usar con cepillo dental o con bandejas específicas.
+Presentación económica: Envase de 175g, ideal para múltiples aplicaciones.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734709189/DESMANCHADOR_EN_POLVO_yyx2qo.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desmingel Jeringa 10ml </t>
+  </si>
+  <si>
+    <t>La Desmingel Jeringa 10ml es una solución de gel diseñada para procedimientos odontológicos específicos. Este producto es ideal para ser utilizado en tratamientos de limpieza, desinfección y en la preparación de cavidades dentales antes de aplicar otros tratamientos. Su formato en jeringa facilita su aplicación controlada, proporcionando precisión y comodidad para el profesional odontológico durante las intervenciones.</t>
+  </si>
+  <si>
+    <t>Presentación: Jeringa de 10ML.
+Uso: Utilizada para la limpieza y desinfección en tratamientos odontológicos.
+Composición: Gel con propiedades desinfectantes, recomendado para procedimientos dentales.
+Aplicación: Sencilla y precisa, ideal para la administración de geles en cavidades dentales o durante la preparación de tratamientos odontológicos.
+Indicaciones: Es adecuada para el uso de higienización y preparación de cavidades en procedimientos como obturaciones, endodoncias, y otros tratamientos dentales.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734709575/DESMIGEL_qklxbg.png</t>
+  </si>
+  <si>
+    <t>Enhebradores Plásticos 24un</t>
+  </si>
+  <si>
+    <t>Los Enhebradores Plásticos 24un son herramientas de alta calidad diseñadas para facilitar el enhebrado de hilos en procedimientos odontológicos. Cada paquete contiene 24 unidades, ideales para clínicas dentales que requieren productos duraderos y fáciles de usar en diversos tratamientos. Estos enhebradores plásticos son perfectos para procedimientos de ortodoncia, limpieza interdental, y otros cuidados odontológicos.</t>
+  </si>
+  <si>
+    <t>Contenido: Paquete de 24 unidades.
+Material: Plástico resistente y de alta calidad.
+Diseño: Ergonómico y fácil de usar, diseñado para facilitar la manipulación durante los procedimientos odontológicos.
+Uso: Ideal para el enhebrado de hilos en tratamientos de ortodoncia, higiene interdental, y otros cuidados odontológicos.
+Aplicaciones: Muy útil en clínicas dentales y consultorios odontológicos para una correcta higiene de los pacientes.
+Durabilidad: Plástico de alta resistencia para un uso prolongado.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734709880/ENHEBRADORES_rrl0rb.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enj Bucal Revelador de Placa Proquident 200ml </t>
+  </si>
+  <si>
+    <t>Enjuague Bucal Revelador de Placa Proquident 200ml - Sabor Chicle El enjuague bucal revelador de placa es ideal para mantener una higiene bucal óptima. Su fórmula especial permite identificar fácilmente las zonas de la boca con placa dental, ayudando a mejorar la eficacia del cepillado y prevenir problemas dentales. Con un agradable sabor a chicle, es perfecto para toda la familia, promoviendo una sonrisa más saludable y fresca.</t>
+  </si>
+  <si>
+    <t>Volumen: 200 ml.
+Sabor: Chicle, para una experiencia agradable durante su uso.
+Función principal: Revelador de placa dental, ideal para visualizar las zonas con acumulación de placa y mejorar el cepillado.
+Beneficios: Ayuda a prevenir problemas como caries, gingivitis y mal aliento al detectar áreas donde la placa se acumula.
+Modo de uso: Enjuagar con una pequeña cantidad de enjuague bucal durante 30 segundos a 1 minuto. Se recomienda usar después del cepillado para obtener mejores resultados.
+Apto para: Adultos y niños mayores de 6 años bajo supervisión.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734710177/ENJUAGUE_BUCAL_REVELADOR_DE_PLACA_200ML_eh1ijf.png</t>
+  </si>
+  <si>
+    <t>Enj Bucal Sensitive de 500ml</t>
+  </si>
+  <si>
+    <t>El Enjuague Bucal Sensitive de 500ml con sabor a sandía es un producto especialmente diseñado para ayudar a mantener una higiene bucal eficaz en personas con dientes sensibles. Su fórmula suave limpia y refresca, protegiendo las encías y reduciendo la sensación de incomodidad en los dientes sensibles. Además, su agradable sabor a sandía proporciona una sensación de frescura duradera, haciendo que el cuidado bucal sea más placentero.</t>
+  </si>
+  <si>
+    <t>Tamaño: 500ml
+Sabor: Sandía
+Ideal para dientes sensibles: Diseñado específicamente para reducir la incomodidad asociada con los dientes sensibles.
+Higiene completa: Ayuda a eliminar bacterias, previniendo la formación de placa y ofreciendo una protección adicional a las encías.
+Frescura duradera: Proporciona una sensación de frescura en la boca durante todo el día.
+Uso diario: Perfecto para complementar el cepillado y mantener una salud bucal óptima.
+Fórmula suave: No irrita las encías y es adecuado para quienes sufren de sensibilidad dental.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734710898/ENJUAGUE_SENSITVE_500ML_ctrvie.png</t>
+    </r>
+  </si>
+  <si>
+    <t>Eugenol 15ML USP</t>
+  </si>
+  <si>
+    <t>Eugenol 15ML USP es un líquido de alta calidad utilizado en procedimientos odontológicos como anestesia, tratamiento de conductos radiculares y en la fabricación de materiales de impresión y restauración. Su pureza y efectividad lo convierten en una opción confiable para dentistas y profesionales del sector.</t>
+  </si>
+  <si>
+    <t>Composición: Eugenol puro (15ML USP).
+Uso principal: Utilizado como base para cementos temporales y permanentes, en tratamientos de conductos radiculares y para aliviar el dolor postoperatorio.
+Presentación: Frasco de 15ML.
+Propiedades: Propiedades anestésicas locales, efecto antiséptico y calmante, ayuda a reducir la inflamación y el dolor, compatible con materiales de restauración odontológica.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734711232/EUGENOL_yozzks.png</t>
+    </r>
+  </si>
+  <si>
+    <t>Flosser Adulto 40un</t>
+  </si>
+  <si>
+    <t>Flosser Adulto es un producto diseñado para mantener una higiene bucal óptima. Con su diseño práctico y ergonómico, cada flosser está especialmente formulado para facilitar la limpieza entre los dientes, eliminando restos de comida y placa bacteriana, ayudando a prevenir problemas dentales como las caries y la gingivitis. Viene en un paquete de 40 unidades, ideal para su uso diario, permitiendo mantener una sonrisa saludable en todo momento.</t>
+  </si>
+  <si>
+    <t>Cantidad: 40 unidades por paquete.
+Diseño ergonómico: Comodidad y facilidad de uso, especialmente diseñado para adultos.
+Cerdas finas: Ayuda a remover eficazmente los residuos de comida y la placa interdental.
+Fácil de usar: Perfecto para limpiar entre los dientes de manera rápida y sencilla.
+Previene problemas bucales: Reduce el riesgo de caries y gingivitis al mantener las encías saludables.
+Ideal para uso diario: Práctico para llevar en la bolsa o dejar en casa para su uso regular.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734711573/FLOSSER_ADULTO_hs1auy.png</t>
+  </si>
+  <si>
+    <t>Flosser Kids 40un</t>
+  </si>
+  <si>
+    <t>Flosser Kids es un hilo dental especialmente diseñado para niños. Viene en una presentación de 40 unidades, proporcionando una forma fácil y efectiva de mantener la salud dental de los más pequeños. Gracias a su diseño amigable y suave, el hilo dental Flosser Kids facilita la limpieza entre los dientes, ayudando a eliminar los restos de comida y la placa bacteriana, lo que previene la caries y mejora la salud bucal de los niños.</t>
+  </si>
+  <si>
+    <t>Diseño especial para niños: El hilo dental está diseñado con una textura suave y agradable para niños, lo que hace que el uso sea más cómodo.
+Fácil de usar: Presentación práctica en forma de hilo dental pre-cortado, ideal para que los niños lo utilicen de manera autónoma o con la ayuda de un adulto.
+Eliminación de restos de comida: Ayuda a limpiar entre los dientes, eliminando residuos que el cepillo no puede alcanzar.
+Prevención de caries: Favorece la prevención de caries y otras enfermedades bucales al promover una higiene bucal completa.
+40 unidades por paquete: Cada paquete contiene 40 hilos dentales individuales, ideales para uso diario.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734711766/FLOSSERS_KIDS_gdocmr.png</t>
+  </si>
+  <si>
+    <t>Glutacides LIimón 3800ml</t>
+  </si>
+  <si>
+    <t>Glutacides LIimón es un desinfectante de uso odontológico, desarrollado especialmente para la limpieza y desinfección de superficies en consultorios y equipos dentales. Su fórmula eficaz garantiza una acción antimicrobiana potente que elimina virus, bacterias y hongos, asegurando un ambiente de trabajo limpio y seguro. Su agradable fragancia a limón contribuye a mantener el espacio libre de olores desagradables, ofreciendo una sensación fresca.</t>
+  </si>
+  <si>
+    <t>Volumen: 3800ml, ideal para el uso prolongado en consultorios odontológicos.
+Acción Antimicrobiana: Elimina virus, bacterias y hongos, protegiendo tanto a los pacientes como al personal.
+Fórmula de Alta Eficacia: Asegura una limpieza profunda de superficies de trabajo, equipos odontológicos y mobiliario.
+Fragancia a Limón: Aporta un ambiente fresco y agradable, reduciendo los malos olores en el consultorio.
+Fácil de Usar: Ideal para rociar sobre superficies, facilitando una rápida y eficiente desinfección.
+Uso Profesional: Especialmente diseñado para consultorios dentales y centros odontológicos.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734711963/GLUTACIDES_3.8L_dlp4oo.png</t>
+  </si>
+  <si>
+    <t>Glutacides LIimón 1000ml</t>
+  </si>
+  <si>
+    <t>Volumen: 1000ml
+Acción Antimicrobiana: Elimina virus, bacterias y hongos, protegiendo tanto a los pacientes como al personal.
+Fórmula de Alta Eficacia: Asegura una limpieza profunda de superficies de trabajo, equipos odontológicos y mobiliario.
+Fragancia a Limón: Aporta un ambiente fresco y agradable, reduciendo los malos olores en el consultorio.
+Fácil de Usar: Ideal para rociar sobre superficies, facilitando una rápida y eficiente desinfección.
+Uso Profesional: Especialmente diseñado para consultorios dentales y centros odontológicos.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734712284/GLUTACIDES_1000ML_jvntid.png</t>
+  </si>
+  <si>
+    <t>Gotas Reveladoras de Placa Bacteriana</t>
+  </si>
+  <si>
+    <t>Las Gotas Reveladoras de Placa Bacteriana son un innovador producto de uso odontológico que permite a los profesionales de la salud dental identificar y visualizar la placa bacteriana en los dientes de manera rápida y sencilla. Estas gotas, al ser aplicadas sobre los dientes, tiñen la placa bacteriana, facilitando la detección de áreas que necesitan una limpieza más profunda. Son una herramienta útil para la educación del paciente sobre la importancia de una correcta</t>
+  </si>
+  <si>
+    <t>Presentación: 10 ml.
+Marca: Proquident.
+Función: Revela la placa bacteriana en los dientes al teñirla temporalmente.
+Fácil aplicación: Solo requiere unas pocas gotas para observar la placa bacteriana en la superficie dental.
+Educativo: Ayuda a los pacientes a identificar las áreas de la boca que requieren atención especial durante el cepillado.
+Uso profesional y doméstico: Ideal para dentistas y también recomendado para uso en casa bajo supervisión.
+Sin efectos secundarios: Totalmente seguro para el uso dental y no irritante para las encías.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734712393/GOTAS_REVELADORAS_10ML_tpimru.png</t>
+    </r>
+  </si>
+  <si>
+    <t>El hemostático 15ml</t>
+  </si>
+  <si>
+    <t>El hemostático 15ml es un líquido especializado para el control del sangrado durante procedimientos odontológicos. Su fórmula de acción rápida ayuda a coagular la sangre de manera eficiente, facilitando una curación más rápida y segura tras intervenciones quirúrgicas en la boca. Es especialmente útil durante extracciones dentales, tratamientos periodontales, y otras cirugías dentales, asegurando que el procedimiento sea lo más limpio y efectivo posible.</t>
+  </si>
+  <si>
+    <t>Contenido: 15ml.
+Uso: Control del sangrado durante procedimientos odontológicos.
+Modo de acción: Ayuda a coagular rápidamente la sangre, reduciendo el tiempo de sangrado y mejorando el proceso de cicatrización.
+Aplicación: Ideal para extracciones dentales, cirugía periodontal, y otras intervenciones quirúrgicas en la cavidad bucal.
+Ventajas: Fórmula eficaz y segura para el control de hemorragias menores en la práctica odontológica.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734712718/HEMOSTATICO_dccmnu.png</t>
+  </si>
+  <si>
+    <t>Hidróxido de Calcio 7g</t>
+  </si>
+  <si>
+    <t>Hidróxido de Calcio 7g es un producto odontológico utilizado principalmente para la protección pulpar y el tratamiento de conductos radiculares. Este material tiene propiedades antibacterianas, estimula la formación de dentina secundaria y ayuda en la reparación de tejidos dentales, ofreciendo una solución eficaz y segura en tratamientos endodónticos.</t>
+  </si>
+  <si>
+    <t>Presentación: 7g
+Uso principal: Tratamientos de conductos radiculares, protección de la pulpa dental, y como base en cavidades.
+Composición: Hidróxido de calcio en polvo, ideal para mezclarse con agua o una solución adecuada antes de su aplicación.
+Indicado para: Endodoncia, tratamientos de conductos radiculares y reparación de lesiones pulpares.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734712967/HIDROXIDO_DE_CALCIO_t6o8o7.png</t>
+  </si>
+  <si>
+    <t>Hilo Retractor</t>
+  </si>
+  <si>
+    <t>El Hilo Retractor 2m es un producto de alta calidad diseñado especialmente para la práctica odontológica, utilizado en procedimientos de ortodoncia y cirugía periodontal. Este hilo permite retraer eficazmente los tejidos blandos alrededor de los dientes, creando el espacio necesario para que el dentista pueda realizar intervenciones con mayor precisión. Ideal para tratamientos de colocación de coronas, impresiones dentales y otros procedimientos ortodónticos.</t>
+  </si>
+  <si>
+    <t>Longitud: 2 metros
+Composición: Hilo de alta resistencia y flexibilidad
+Uso principal: Retracción de los tejidos gingivales en procedimientos ortodónticos
+Presentación: Envase compacto para fácil manipulación y almacenamiento
+Ventajas: Su diseño flexible y resistente permite un manejo fácil y efectivo, adaptándose a la anatomía del paciente sin causar incomodidad.
+Indicaciones: Ideal para odontólogos y ortodoncistas en la colocación de coronas, puentes y en la toma de impresiones.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734713751/HILO_RETRACTOR_rtzvfa.png</t>
+  </si>
+  <si>
+    <t>Kit de Ortodoncia Blister</t>
+  </si>
+  <si>
+    <t>El Kit de Ortodoncia Blister es un conjunto completo de productos diseñados para facilitar la higiene bucal en personas que utilizan brackets u otros dispositivos ortodónticos. Este kit contiene todo lo necesario para prevenir la acumulación de placa y mantener una boca saludable durante el tratamiento, incluyendo crema dental para dientes sensibles, cera protectora, y herramientas específicas para una limpieza profunda y cómoda.
+Este producto es ideal tanto para adolescentes como para adultos que buscan un cuidado bucal óptimo durante su tratamiento ortodóntico.</t>
+  </si>
+  <si>
+    <t>Crema dental para dientes sensibles: Ayuda a reducir la sensibilidad dental común en tratamientos de ortodoncia.
+Cepillo de ortodoncia: Diseñado específicamente para limpiar eficazmente alrededor de los brackets.
+Seda dental con cera (12 metros): Facilita la limpieza interdental, incluso en áreas de difícil acceso.
+Cera ortodóntica: Protege los tejidos bucales de las irritaciones causadas por los brackets.
+Enhebradores e interproximales antibacteriales: Herramientas ideales para limpiar entre dientes y aparatos.
+Gotas reveladoras de placa bacteriana: Ayudan a identificar áreas donde se acumula la placa para mejorar la técnica de cepillado.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734796941/KIT_DE_ORTODONCIA_BLISTER_aflphn.png</t>
+    </r>
+  </si>
+  <si>
+    <t>Óxido de Zinc 10g</t>
+  </si>
+  <si>
+    <t>El óxido de zinc es un material esencial en odontología, ideal para una amplia variedad de aplicaciones clínicas y restaurativas. Este producto de alta calidad, fabricado por Proquident, es indispensable en procedimientos odontológicos gracias a sus propiedades antimicrobianas, adhesivas y de sellado.</t>
+  </si>
+  <si>
+    <t>Composición: Óxido de zinc puro, presentado en polvo fino para facilitar la mezcla y aplicación.
+Uso odontológico: Ideal para preparar cementos y bases intermedias en restauraciones temporales y definitivas.
+Compatibilidad: Compatible con diferentes tipos de líquidos, como eugenol, para formar pastas de sellado o cementado.
+Propiedades antimicrobianas: Ayuda a reducir el riesgo de infecciones.
+Presentación: Envase práctico de 10g, con cierre hermético para mantener la frescura del producto.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734797570/OXIDO_DE_ZINC_10G_vubgsd.png</t>
+    </r>
+  </si>
+  <si>
+    <t>Pasta Profiláctica 60g</t>
+  </si>
+  <si>
+    <t>La pasta profiláctica es un producto esencial en la práctica odontológica, diseñado para eliminar la placa dental y las manchas superficiales de manera eficiente. Con su fórmula especializada, fabricada por Proquident, garantiza resultados efectivos durante la profilaxis dental, dejando los dientes limpios y con un acabado brillante.</t>
+  </si>
+  <si>
+    <t>Composición especializada: Contiene abrasivos suaves para una limpieza profunda pero no invasiva.
+Propiedades pulidoras: Ideal para eliminar manchas superficiales y devolver el brillo natural a los dientes.
+Presentación práctica: Envase de 60g, fácil de almacenar y usar durante las sesiones de limpieza.
+Sabor agradable: Disponible en sabores suaves que proporcionan una experiencia cómoda al paciente.
+Uso profesional: Recomendado para procedimientos de limpieza dental realizados por odontólogos e higienistas dentales.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734797814/PASTA_PROFILACTICA_gmgotn.png</t>
+  </si>
+  <si>
+    <t>Enjuague Bucal Zero 500ml</t>
+  </si>
+  <si>
+    <t>El enjuague bucal Zero de Proquident es una solución diseñada para complementar la higiene oral diaria. Con su fórmula avanzada sin alcohol, brinda una limpieza profunda y ayuda a mantener el equilibrio natural de la boca, siendo ideal para personas con sensibilidad o que prefieren un cuidado suave pero efectivo.</t>
+  </si>
+  <si>
+    <t>Fórmula sin alcohol: No irrita las encías ni genera ardor, ideal para personas con sensibilidad bucal.
+Propiedades antisépticas: Ayuda a eliminar bacterias, reduciendo el riesgo de caries y enfermedades periodontales.
+Fresco aliento: Deja una sensación de frescura prolongada gracias a su suave sabor mentolado.
+Uso diario: Perfecto para complementar el cepillado, proporcionando protección adicional contra la acumulación de placa.
+Presentación práctica: Botella de 500ml, diseñada para un fácil almacenamiento y uso prolongado.
+Recomendado por expertos: Producto respaldado por Proquident, líder en innovación y calidad en el cuidado oral.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734798668/PROQUIDENT_ENJUAGUE_BUCAL_ZERO_500ML_ip6jfu.png</t>
+  </si>
+  <si>
+    <t>Enjuague Bucal Zero 1000ml</t>
+  </si>
+  <si>
+    <t>Fórmula sin alcohol: No irrita las encías ni genera ardor, ideal para personas con sensibilidad bucal.
+Propiedades antisépticas: Ayuda a eliminar bacterias, reduciendo el riesgo de caries y enfermedades periodontales.
+Fresco aliento: Deja una sensación de frescura prolongada gracias a su suave sabor mentolado.
+Uso diario: Perfecto para complementar el cepillado, proporcionando protección adicional contra la acumulación de placa.
+Presentación: Botella de 1000ml.
+Recomendado por expertos: Producto respaldado por Proquident, líder en innovación y calidad en el cuidado oral.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734799335/pROQUIDENT_ENJUAGUE_BUCAL_ZERO_1000ML_lbl0b3.png</t>
+  </si>
+  <si>
+    <t>Detergente Multienzimático 3800ml</t>
+  </si>
+  <si>
+    <t>Proquizyme es un detergente multienzimático diseñado específicamente para la limpieza profunda de instrumental y equipos odontológicos. Su avanzada fórmula enzimática asegura la remoción efectiva de residuos orgánicos como sangre, proteínas y otros restos biológicos, protegiendo y alargando la vida útil del instrumental.</t>
+  </si>
+  <si>
+    <t>Fórmula avanzada: Contiene múltiples enzimas (proteasas, lipasas y amilasas) que garantizan la eliminación eficiente de restos orgánicos.
+Aplicación profesional: Ideal para la limpieza de instrumentos quirúrgicos, odontológicos y equipos como turbinas, fresas y bandejas metálicas.
+Presentación: Envase de 3800 ml con sistema de dosificación fácil, diseñado para clínicas y consultorios con alta demanda de limpieza.
+Biodegradable: Producto amigable con el medio ambiente, sin residuos tóxicos.
+Compatibilidad: Seguro para utilizar en acero inoxidable, plásticos y materiales delicados del instrumental.
+Efectividad rápida: Reduce el tiempo necesario para la limpieza, permitiendo mayor productividad en los procedimientos clínicos.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734799635/PROQUIZYME_3.8L_injnux.png</t>
+    </r>
+  </si>
+  <si>
+    <t>Desinfectante de Dispositivos Médicos 240ml</t>
+  </si>
+  <si>
+    <t>El desinfectante Proquizyme de Proquident es una solución altamente efectiva y especializada para la limpieza y desinfección de dispositivos médicos y equipos odontológicos. Formulado para eliminar microorganismos, bacterias y hongos, garantiza una limpieza profunda y segura, prolongando la vida útil de los instrumentos.</t>
+  </si>
+  <si>
+    <t>Eficiencia comprobada: Acción rápida y efectiva contra una amplia gama de microorganismos, incluyendo bacterias y hongos.
+Compatibilidad: Diseñado específicamente para dispositivos médicos y odontológicos, sin riesgo de corrosión ni daños.
+Fácil de usar: Fórmula lista para usar, no requiere dilución.
+Capacidad: Presentación en envase de 240 ml, ideal para clínicas y consultorios.
+Certificación: Cumple con las normativas de calidad para productos de uso médico y odontológico.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734800041/PROQUIZYME_240_ccehwh.png</t>
+    </r>
+  </si>
+  <si>
+    <t>Detergente Multienzimático 100ml</t>
+  </si>
+  <si>
+    <t>El detergente multienzimático PROQUIZYME es un producto avanzado diseñado para garantizar una limpieza eficaz y segura de instrumentos y equipos odontológicos. Su fórmula especializada con múltiples enzimas elimina residuos orgánicos de manera eficiente, protegiendo al mismo tiempo los materiales delicados de tus instrumentos.</t>
+  </si>
+  <si>
+    <t>Fórmula multienzimática: Contiene una combinación de enzimas como proteasas, amilasas y lipasas para descomponer residuos orgánicos como proteínas, almidones y grasas.
+Compatibilidad: Ideal para usar en instrumentos metálicos, de vidrio y plástico, así como en equipos automáticos de limpieza por ultrasonido.
+Presentación compacta: Envase de 100 ml fácil de manejar y almacenar.
+Alta eficacia: Garantiza la limpieza profunda de instrumentos quirúrgicos y odontológicos.
+Uso profesional: Recomendado para clínicas odontológicas, laboratorios y entornos hospitalarios.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734801619/PROQUIZYME_PLUS_100_ML_r41sis.png</t>
+    </r>
+  </si>
+  <si>
+    <t>Detergente Multienzimático 500ml</t>
+  </si>
+  <si>
+    <t>Fórmula multienzimática: Contiene una combinación de enzimas como proteasas, amilasas y lipasas para descomponer residuos orgánicos como proteínas, almidones y grasas.
+Compatibilidad: Ideal para usar en instrumentos metálicos, de vidrio y plástico, así como en equipos automáticos de limpieza por ultrasonido.
+Presentación: Envase de 500 ml.
+Alta eficacia: Garantiza la limpieza profunda de instrumentos quirúrgicos y odontológicos.
+Uso profesional: Recomendado para clínicas odontológicas, laboratorios y entornos hospitalarios.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734802191/PROQUIZYME_PLUS_500ML_flfboj.png</t>
+    </r>
+  </si>
+  <si>
+    <t>Seda Dental 50 mts</t>
+  </si>
+  <si>
+    <t>La Seda Dental con Cera Natural Proquident es una herramienta esencial para la higiene bucal diaria, diseñada para remover eficazmente los restos de alimentos y placa bacteriana de los espacios interdentales. Su fórmula con cera natural y sabor a menta proporciona una experiencia de limpieza cómoda y refrescante, ayudando a prevenir caries y problemas de encías.
+Este producto es ideal para personas con tratamientos ortodónticos, coronas o puentes, y para quienes buscan mantener una salud bucal óptima.</t>
+  </si>
+  <si>
+    <t>Longitud: 50 metros de seda dental de alta calidad, suficiente para un uso prolongado.
+Con cera natural: Facilita el deslizamiento suave entre los dientes, evitando molestias o daños en las encías.
+Sabor a menta: Proporciona una sensación de frescura y limpieza duradera.
+Elimina la placa bacteriana: Ayuda a prevenir la formación de caries y enfermedades periodontales.
+Fácil de usar: Diseño práctico y compacto que permite llevarlo a cualquier lugar.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734802735/SEDA_DENTAL_50MTS_fqnqod.png</t>
+    </r>
+  </si>
+  <si>
+    <t>Seda Dental 400 mts</t>
+  </si>
+  <si>
+    <t>Longitud: 400 metros de seda dental de alta calidad, suficiente para un uso prolongado.
+Con cera natural: Facilita el deslizamiento suave entre los dientes, evitando molestias o daños en las encías.
+Sabor a menta: Proporciona una sensación de frescura y limpieza duradera.
+Elimina la placa bacteriana: Ayuda a prevenir la formación de caries y enfermedades periodontales.
+Fácil de usar: Diseño práctico y compacto que permite llevarlo a cualquier lugar.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734803006/SEDA_DENTAL_400MTS_sk57ph.png</t>
+    </r>
+  </si>
+  <si>
+    <t>El enjuague bucal Zero de Sonrident, fabricado por Proquident, es la elección ideal para una higiene bucal completa y refrescante. Diseñado para cuidar la salud bucal de manera delicada, este producto no contiene alcohol, lo que lo hace apto para personas con sensibilidad oral.</t>
+  </si>
+  <si>
+    <t>Sin alcohol: Fórmula suave que no irrita ni reseca la cavidad bucal.
+Propiedades antibacterianas: Ayuda a eliminar las bacterias que causan el mal aliento y enfermedades periodontales.
+Frescura prolongada: Proporciona un aliento fresco y duradero.
+Protección integral: Ayuda a prevenir caries, gingivitis y placa bacteriana.
+Tamaño práctico: Botella de 500ml ideal para uso diario en casa o en consultorios odontológicos.
+Apto para todos: Especialmente recomendado para personas con sensibilidad oral o que evitan productos con alcohol.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734803531/sonrident_enjuague_zero_500ml_nx0o6c.png</t>
+    </r>
+  </si>
+  <si>
+    <t>Tiras de Myllar 50un</t>
+  </si>
+  <si>
+    <t>Las tiras de Myllar son un insumo dental de alta calidad utilizado principalmente en odontología restaurativa. Estas tiras se emplean para crear una barrera eficaz durante el proceso de obturación de cavidades, ayudando a moldear y dar forma a los empastes. Con su alta resistencia y flexibilidad, permiten un trabajo preciso y seguro en diversos procedimientos dentales.</t>
+  </si>
+  <si>
+    <t>Composición: Material flexible y resistente, diseñado para soportar la presión durante la restauración de cavidades dentales.
+Cantidad: 50 unidades por paquete, ideal para varios tratamientos.
+Uso odontológico: Utilizadas para la colocación de empastes en dientes posteriores o anteriores, proporcionando una mejor adaptación del material restaurador.
+Fácil manejo: Las tiras son delgadas y flexibles, lo que permite al odontólogo trabajar con precisión, asegurando un ajuste adecuado del material.
+Alta calidad: Fabricadas por Proquident, garantizando una durabilidad y efectividad en su uso en el consultorio odontológico.
+Aplicación: Se emplean en la creación de un espacio limpio y preciso durante la colocación de empastes y restauraciones.
+Presentación: Empaque con 50 unidades para facilitar el uso en múltiples procedimientos.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734803725/TIRAS_DE_MYLLAR_kwgs7m.png</t>
+    </r>
+  </si>
+  <si>
+    <t>Xilodent 20ml</t>
+  </si>
+  <si>
+    <t>Xilodent es un gel anestésico de uso profesional en odontología, especialmente formulado para proporcionar alivio temporal del dolor durante procedimientos odontológicos. Su formulación con xilocaína permite adormecer eficazmente las áreas tratadas, facilitando una experiencia sin dolor para el paciente. Este gel es ideal para ser utilizado antes de intervenciones como la extracción de piezas dentales, limpieza profunda y otros procedimientos restaurativos.</t>
+  </si>
+  <si>
+    <t>Composición: Contiene xilocaína (lidocaína) al 2%, que es un potente anestésico local utilizado comúnmente en odontología.
+Presentación: Viene en un práctico envase de 20 ml, ideal para uso clínico y de fácil aplicación.
+Acción rápida: El gel tiene un inicio de acción rápido, proporcionando un alivio inmediato y duradero en las áreas tratadas.
+Uso seguro: Diseñado para ser utilizado únicamente por profesionales de la salud dental, siguiendo las indicaciones para garantizar la seguridad del paciente.
+Eficiencia: Ideal para procedimientos restaurativos que requieren un adormecimiento preciso de los tejidos blandos, como la preparación para coronas, obturaciones, o extracciones.
+Compatibilidad: Compatible con otros productos odontológicos y procedimientos sin interferir en la eficacia de los mismos.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734803913/XILODENT_geenhy.png</t>
+  </si>
+  <si>
+    <t>Zonident 5% 1000ml</t>
+  </si>
+  <si>
+    <t>Zonident es un desinfectante de uso odontológico, formulado para ser utilizado en la limpieza y desinfección de instrumental dental y superficies en clínicas odontológicas. Su concentración al 5% lo convierte en una opción eficaz para eliminar bacterias y microorganismos, asegurando un entorno seguro y libre de contaminación durante los tratamientos.</t>
+  </si>
+  <si>
+    <t>Composición: Solución al 5% de clorhexidina, un agente antiséptico de amplio espectro.
+Presentación: Envase de 1000ml, ideal para clínicas dentales con alta demanda de desinfección.
+Eficiencia antimicrobiana: Eficaz contra bacterias, hongos y algunos virus, proporcionando una desinfección de alto nivel.
+Uso clínico: Recomendado para la desinfección de superficies de trabajo, instrumental y equipos odontológicos, asegurando la higiene antes, durante y después de cada procedimiento.
+Aplicación: Puede ser utilizado en la limpieza de la cavidad bucal de los pacientes para reducir la carga bacteriana durante procedimientos quirúrgicos o tratamientos invasivos.
+Seguro para el ambiente clínico: No daña el equipo ni las superficies si se utiliza correctamente.
+Certificación de calidad: Producto fabricado por Proquident, una marca confiable en el campo de la odontología.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734804080/ZONIDENT_100ML_k3oerk.png</t>
+    </r>
+  </si>
+  <si>
+    <t>Zonident 5% 120ml</t>
+  </si>
+  <si>
+    <t>Composición: Solución al 5% de clorhexidina, un agente antiséptico de amplio espectro.
+Presentación: Envase de 120m.
+Eficiencia antimicrobiana: Eficaz contra bacterias, hongos y algunos virus, proporcionando una desinfección de alto nivel.
+Uso clínico: Recomendado para la desinfección de superficies de trabajo, instrumental y equipos odontológicos, asegurando la higiene antes, durante y después de cada procedimiento.
+Aplicación: Puede ser utilizado en la limpieza de la cavidad bucal de los pacientes para reducir la carga bacteriana durante procedimientos quirúrgicos o tratamientos invasivos.
+Seguro para el ambiente clínico: No daña el equipo ni las superficies si se utiliza correctamente.
+Certificación de calidad: Producto fabricado por Proquident, una marca confiable en el campo de la odontología.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734804268/ZONIDENT_120_hj7afb.png</t>
+  </si>
+  <si>
+    <t>Zonident 5% 3800ml</t>
+  </si>
+  <si>
+    <t>Composición: Solución al 5% de clorhexidina, un agente antiséptico de amplio espectro.
+Presentación: Envase de 3800ml, ideal para clínicas dentales con alta demanda de desinfección.
+Eficiencia antimicrobiana: Eficaz contra bacterias, hongos y algunos virus, proporcionando una desinfección de alto nivel.
+Uso clínico: Recomendado para la desinfección de superficies de trabajo, instrumental y equipos odontológicos, asegurando la higiene antes, durante y después de cada procedimiento.
+Aplicación: Puede ser utilizado en la limpieza de la cavidad bucal de los pacientes para reducir la carga bacteriana durante procedimientos quirúrgicos o tratamientos invasivos.
+Seguro para el ambiente clínico: No daña el equipo ni las superficies si se utiliza correctamente.
+Certificación de calidad: Producto fabricado por Proquident, una marca confiable en el campo de la odontología.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734804304/ZONIDENT_GALON_kqokqy.png</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -517,6 +1374,11 @@
       <color rgb="FF0000FF"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -532,7 +1394,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border/>
     <border>
       <left style="thin">
@@ -660,11 +1522,53 @@
         <color rgb="FFF6F8F9"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF284E3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFF6F8F9"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF6F8F9"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF284E3F"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF6F8F9"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFF6F8F9"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF6F8F9"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF284E3F"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF6F8F9"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF284E3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF6F8F9"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF284E3F"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="25">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -725,6 +1629,21 @@
     <xf borderId="6" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -783,7 +1702,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I29" displayName="Productos" name="Productos" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I73" displayName="Productos" name="Productos" id="1">
+  <autoFilter ref="$A$1:$I$73"/>
   <tableColumns count="9">
     <tableColumn name="id" id="1"/>
     <tableColumn name="nombre" id="2"/>
@@ -1700,7 +2620,7 @@
         <v>111</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>112</v>
+        <v>12</v>
       </c>
       <c r="F26" s="14" t="s">
         <v>13</v>
@@ -1709,7 +2629,7 @@
         <v>14</v>
       </c>
       <c r="I26" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27">
@@ -1717,26 +2637,26 @@
         <v>26.0</v>
       </c>
       <c r="B27" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="D27" s="10" t="s">
         <v>115</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>116</v>
       </c>
       <c r="E27" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G27" s="10" t="s">
         <v>14</v>
       </c>
       <c r="H27" s="12"/>
       <c r="I27" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28">
@@ -1744,26 +2664,1196 @@
         <v>27.0</v>
       </c>
       <c r="B28" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C28" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="D28" s="6" t="s">
         <v>120</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>121</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>51</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>14</v>
       </c>
       <c r="H28" s="7"/>
       <c r="I28" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="20">
+        <v>28.0</v>
+      </c>
+      <c r="B29" s="11" t="s">
         <v>122</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="21">
+        <v>29.0</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I30" s="16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="20">
+        <v>30.0</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I31" s="18" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="21">
+        <v>31.0</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="G32" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I32" s="16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="20">
+        <v>32.0</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="21">
+        <v>33.0</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G34" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I34" s="16" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="20">
+        <v>34.0</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="21">
+        <v>35.0</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G36" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I36" s="16" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="20">
+        <v>36.0</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I37" s="17" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="21">
+        <v>37.0</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G38" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I38" s="19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="20">
+        <v>38.0</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I39" s="17" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="21">
+        <v>39.0</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G40" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I40" s="19" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="20">
+        <v>40.0</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I41" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="21">
+        <v>41.0</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G42" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I42" s="19" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="20">
+        <v>42.0</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I43" s="17" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="21">
+        <v>43.0</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G44" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I44" s="19" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="20">
+        <v>44.0</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="G45" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I45" s="17" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="21">
+        <v>45.0</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F46" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G46" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I46" s="19" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="20">
+        <v>46.0</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="G47" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I47" s="13" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="21">
+        <v>47.0</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>201</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G48" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I48" s="16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="20">
+        <v>48.0</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="G49" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I49" s="17" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="21">
+        <v>49.0</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G50" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I50" s="19" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="20">
+        <v>50.0</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="G51" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I51" s="17" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="21">
+        <v>51.0</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G52" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I52" s="19" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="20">
+        <v>52.0</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="G53" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I53" s="13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="21">
+        <v>53.0</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="E54" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F54" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G54" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I54" s="19" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="20">
+        <v>54.0</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="E55" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F55" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="G55" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I55" s="17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="21">
+        <v>55.0</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="D56" s="14" t="s">
+        <v>232</v>
+      </c>
+      <c r="E56" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="F56" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G56" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I56" s="19" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="20">
+        <v>56.0</v>
+      </c>
+      <c r="B57" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="E57" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F57" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="G57" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I57" s="13" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="21">
+        <v>57.0</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>239</v>
+      </c>
+      <c r="D58" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="E58" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F58" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G58" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I58" s="16" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="20">
+        <v>58.0</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="E59" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="G59" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I59" s="17" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="21">
+        <v>59.0</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="D60" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="E60" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="F60" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G60" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I60" s="19" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="20">
+        <v>60.0</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="E61" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F61" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="G61" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I61" s="17" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="21">
+        <v>61.0</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="D62" s="14" t="s">
+        <v>255</v>
+      </c>
+      <c r="E62" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F62" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G62" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I62" s="16" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="20">
+        <v>62.0</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="D63" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="E63" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F63" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="G63" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I63" s="13" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="21">
+        <v>63.0</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="D64" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="E64" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F64" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G64" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I64" s="16" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="20">
+        <v>64.0</v>
+      </c>
+      <c r="B65" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="C65" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="E65" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F65" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="G65" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I65" s="13" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="21">
+        <v>65.0</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="D66" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="E66" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="F66" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G66" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I66" s="16" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="20">
+        <v>66.0</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="D67" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="E67" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F67" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="G67" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I67" s="13" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="21">
+        <v>67.0</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>275</v>
+      </c>
+      <c r="D68" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="E68" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="F68" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G68" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I68" s="16" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="20">
+        <v>68.0</v>
+      </c>
+      <c r="B69" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="C69" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="E69" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F69" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="G69" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I69" s="13" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="21">
+        <v>69.0</v>
+      </c>
+      <c r="B70" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="C70" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="D70" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="E70" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F70" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G70" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I70" s="19" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="20">
+        <v>70.0</v>
+      </c>
+      <c r="B71" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="C71" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="E71" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F71" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="G71" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I71" s="13" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="21">
+        <v>71.0</v>
+      </c>
+      <c r="B72" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="C72" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="D72" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="E72" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F72" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="G72" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I72" s="19" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="22">
+        <v>72.0</v>
+      </c>
+      <c r="B73" s="23" t="s">
+        <v>293</v>
+      </c>
+      <c r="C73" s="23" t="s">
+        <v>287</v>
+      </c>
+      <c r="D73" s="23" t="s">
+        <v>294</v>
+      </c>
+      <c r="E73" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F73" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="G73" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I73" s="24" t="s">
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -1795,10 +3885,55 @@
     <hyperlink r:id="rId25" ref="I26"/>
     <hyperlink r:id="rId26" ref="I27"/>
     <hyperlink r:id="rId27" ref="I28"/>
+    <hyperlink r:id="rId28" ref="I29"/>
+    <hyperlink r:id="rId29" ref="I30"/>
+    <hyperlink r:id="rId30" ref="I31"/>
+    <hyperlink r:id="rId31" ref="I32"/>
+    <hyperlink r:id="rId32" ref="I33"/>
+    <hyperlink r:id="rId33" ref="I34"/>
+    <hyperlink r:id="rId34" ref="I35"/>
+    <hyperlink r:id="rId35" ref="I36"/>
+    <hyperlink r:id="rId36" ref="I37"/>
+    <hyperlink r:id="rId37" ref="I38"/>
+    <hyperlink r:id="rId38" ref="I39"/>
+    <hyperlink r:id="rId39" ref="I40"/>
+    <hyperlink r:id="rId40" ref="I41"/>
+    <hyperlink r:id="rId41" ref="I42"/>
+    <hyperlink r:id="rId42" ref="I43"/>
+    <hyperlink r:id="rId43" ref="I44"/>
+    <hyperlink r:id="rId44" ref="I45"/>
+    <hyperlink r:id="rId45" ref="I46"/>
+    <hyperlink r:id="rId46" ref="I47"/>
+    <hyperlink r:id="rId47" ref="I48"/>
+    <hyperlink r:id="rId48" ref="I49"/>
+    <hyperlink r:id="rId49" ref="I50"/>
+    <hyperlink r:id="rId50" ref="I51"/>
+    <hyperlink r:id="rId51" ref="I52"/>
+    <hyperlink r:id="rId52" ref="I53"/>
+    <hyperlink r:id="rId53" ref="I54"/>
+    <hyperlink r:id="rId54" ref="I55"/>
+    <hyperlink r:id="rId55" ref="I56"/>
+    <hyperlink r:id="rId56" ref="I57"/>
+    <hyperlink r:id="rId57" ref="I58"/>
+    <hyperlink r:id="rId58" ref="I59"/>
+    <hyperlink r:id="rId59" ref="I60"/>
+    <hyperlink r:id="rId60" ref="I61"/>
+    <hyperlink r:id="rId61" ref="I62"/>
+    <hyperlink r:id="rId62" ref="I63"/>
+    <hyperlink r:id="rId63" ref="I64"/>
+    <hyperlink r:id="rId64" ref="I65"/>
+    <hyperlink r:id="rId65" ref="I66"/>
+    <hyperlink r:id="rId66" ref="I67"/>
+    <hyperlink r:id="rId67" ref="I68"/>
+    <hyperlink r:id="rId68" ref="I69"/>
+    <hyperlink r:id="rId69" ref="I70"/>
+    <hyperlink r:id="rId70" ref="I71"/>
+    <hyperlink r:id="rId71" ref="I72"/>
+    <hyperlink r:id="rId72" ref="I73"/>
   </hyperlinks>
-  <drawing r:id="rId28"/>
+  <drawing r:id="rId73"/>
   <tableParts count="1">
-    <tablePart r:id="rId30"/>
+    <tablePart r:id="rId75"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Productos densell, gospa, 3m
</commit_message>
<xml_diff>
--- a/data/products.xlsx
+++ b/data/products.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Productos" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Productos!$A$1:$I$73</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Productos!$A$1:$I$93</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="379">
   <si>
     <t>id</t>
   </si>
@@ -1323,12 +1323,472 @@
   <si>
     <t>https://res.cloudinary.com/diqmtzief/image/upload/v1734804304/ZONIDENT_GALON_kqokqy.png</t>
   </si>
+  <si>
+    <t>Filtek Universal Restorative</t>
+  </si>
+  <si>
+    <t>El Filtek Universal Restorative es una resina compuesta de uso universal para restauraciones dentales directas e indirectas. Gracias a su tecnología de nanocompuestos, proporciona alta resistencia, durabilidad y estética natural, siendo ideal para restauraciones en dientes anteriores y posteriores. Este material simplifica los procedimientos clínicos al ofrecer una excelente manejabilidad y una amplia gama de tonos para adaptarse al color de los dientes del paciente.</t>
+  </si>
+  <si>
+    <t>Presentación: Jeringa de 4 gramos.
+Indicaciones: Adecuada para restauraciones en dientes anteriores y posteriores.
+Estética natural: Disponible en tonos que imitan el color natural del diente.
+Alta resistencia: Resistente al desgaste y a las fuerzas de masticación.
+Manejabilidad: Textura suave y no pegajosa para facilitar la colocación y el modelado.
+Tecnología de nanocompuestos: Mejora la estética, resistencia y durabilidad del material.</t>
+  </si>
+  <si>
+    <t>3m</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1736863595/41PBrC2bamL._SL1000__k9ujmx.jpg</t>
+    </r>
+  </si>
+  <si>
+    <t>Filtek Bulk Fill Flowable Restorative</t>
+  </si>
+  <si>
+    <t>El Filtek Bulk Fill Flowable Restorative es una resina compuesta fluida de alta calidad, ideal para restauraciones rápidas y eficientes. Diseñado para ser utilizado como base en restauraciones profundas, este material se adapta perfectamente a las cavidades, garantizando una excelente estética y resistencia. Su fórmula avanzada permite aplicar capas de mayor grosor, reduciendo el tiempo del procedimiento clínico.</t>
+  </si>
+  <si>
+    <t>Presentación: Jeringa con puntas aplicadoras.
+Aplicación en capas de hasta 4 mm: Simplifica el procedimiento restaurativo.
+Fluidez óptima: Asegura una excelente adaptación a las paredes de la cavidad.
+Baja contracción: Minimiza el riesgo de microfiltraciones.
+Resistencia al desgaste: Adecuado para restauraciones en dientes posteriores.
+Compatibilidad universal: Puede usarse con cualquier técnica adhesiva.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1736865220/61b4da17-3fc1-4f7a-8581-8c1458259a0d_cjxdge.jpg</t>
+    </r>
+  </si>
+  <si>
+    <t>Single Bond Universal Adhesive</t>
+  </si>
+  <si>
+    <t>El 3M Single Bond Universal Adhesive es un adhesivo dental universal fotopolimerizable, diseñado para simplificar los procedimientos restaurativos. Este producto ofrece adhesión confiable tanto al esmalte como a la dentina, así como compatibilidad con diversos materiales de restauración, incluyendo resinas compuestas y cerámicas.</t>
+  </si>
+  <si>
+    <t>Versatilidad: Compatible con técnicas de grabado total, autograbado y grabado selectivo, lo que lo hace ideal para diferentes necesidades clínicas.
+Adhesión universal: Funciona de manera eficaz sobre sustratos húmedos o secos, asegurando una fuerte unión al esmalte y la dentina.
+Compatibilidad con múltiples materiales: Es apto para el uso con materiales compuestos, cerámicas, circonio y metales, brindando flexibilidad al profesional.
+Durabilidad: Ofrece una unión resistente que contribuye a la longevidad de las restauraciones dentales.
+Aplicación sencilla: Su presentación en frasco permite un manejo fácil y rápido durante los procedimientos clínicos.
+Reducción de sensibilidad: Diseñado para minimizar la sensibilidad postoperatoria del paciente.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1736866999/DSCF0226_copia_yjkruc.png</t>
+  </si>
+  <si>
+    <t>Resina Filtek Z250 Color B1</t>
+  </si>
+  <si>
+    <t>La Resina Filtek Z250 de 3M es una resina compuesta microhíbrida diseñada para restauraciones dentales directas en dientes anteriores y posteriores. Su fórmula avanzada proporciona excelentes resultados estéticos y funcionales, con una manipulación sencilla y una durabilidad excepcional. Es una elección confiable para odontólogos que buscan combinar calidad, estética y resistencia en sus tratamientos.</t>
+  </si>
+  <si>
+    <t>Fácil manejo: Posee una consistencia óptima que facilita su aplicación y modelado.
+Alta resistencia: Ofrece una excelente resistencia al desgaste y a las fuerzas masticatorias.
+Estética superior: Proporciona una apariencia natural gracias a su color B1, ideal para restauraciones estéticas.
+Versatilidad: Apta para restauraciones en dientes anteriores y posteriores.
+Durabilidad: Garantiza restauraciones duraderas y de alta calidad.
+Fotopolimerizable: Compatible con sistemas de fotopolimerización estándar.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1736869375/DSCF0237_copia__yriays.png</t>
+    </r>
+  </si>
+  <si>
+    <t>Single Bond 2 Adhesive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El Single Bond 2 Adhesive de 3M es un adhesivo dental de fotopolimerización diseñado para garantizar una excelente adhesión en tratamientos restaurativos. Este adhesivo de un solo componente se utiliza junto con resinas compuestas para procedimientos en dientes anteriores y posteriores, ofreciendo una unión confiable al esmalte y la dentina. Es ideal para técnicas de grabado total.
+</t>
+  </si>
+  <si>
+    <t>Fácil aplicación: Formulado para un manejo sencillo y eficiente.
+Alta adhesión: Garantiza una excelente unión entre la estructura dental y la resina compuesta.
+Versatilidad: Compatible con múltiples materiales y sistemas restaurativos.
+Rendimiento confiable: Proporciona una adhesión duradera que mejora los resultados clínicos.
+Transparencia: Su fórmula transparente asegura resultados estéticos sin interferir en la apariencia del material restaurador.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1736869557/DSCF0237_copia_1_bm825q.png</t>
+    </r>
+  </si>
+  <si>
+    <t>Adhesivo Transbond XT Kit x 2 Jeringas</t>
+  </si>
+  <si>
+    <t>El Adhesivo Transbond XT Kit x 2 Jeringas de 3M es un sistema de adhesión fotopolimerizable desarrollado especialmente para la fijación de brackets en tratamientos de ortodoncia. Este adhesivo garantiza una excelente retención y resistencia, asegurando que los brackets permanezcan firmemente adheridos durante todo el tratamiento.
+El Transbond XT es fácil de aplicar y ofrece una consistencia óptima que permite un control preciso durante el posicionamiento de los brackets. Su formulación asegura un curado rápido bajo luz, lo que acelera los procedimientos clínicos.</t>
+  </si>
+  <si>
+    <t>Fotopolimerizable: Se cura rápidamente al exponerse a luz de polimerización, ahorrando tiempo en la consulta.
+Alta retención: Ofrece una adhesión fuerte y duradera para evitar despegues de brackets.
+Fácil de manipular: Consistencia ideal que permite un control preciso durante la aplicación.
+Compatibilidad: Adecuado para utilizar con brackets metálicos, cerámicos y otros materiales.
+Uso clínico: Especialmente diseñado para ortodoncistas en procedimientos de adhesión directa.
+Presentación: Incluye 2 jeringas, asegurando una cantidad suficiente para múltiples tratamientos.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1736870317/Copia_de_DSCF3094-removebg-preview_qekgmr.png</t>
+    </r>
+  </si>
+  <si>
+    <t>Protemp™ 4</t>
+  </si>
+  <si>
+    <t>Protemp™ 4 es un material temporal para restauraciones dentales desarrollado por 3M. Este material es ideal para fabricar restauraciones provisionales como coronas, puentes, carillas e incrustaciones. Diseñado para ofrecer una combinación óptima de resistencia mecánica, estética natural y facilidad de manipulación, este producto garantiza resultados confiables y de alta calidad. El tono A1, visible en la imagen, proporciona una apariencia que se integra de manera natural con los dientes del paciente.</t>
+  </si>
+  <si>
+    <t>Fórmula avanzada: Material a base de resina que ofrece alta resistencia a la abrasión y estabilidad dimensional.
+Presentación en cartuchos: Compatible con pistolas de mezcla automática para una aplicación eficiente.
+Tono disponible: Color A1, ideal para una apariencia estética natural y uniforme.
+Resistencia mecánica superior: Capaz de soportar fuerzas de masticación sin riesgo de fracturas.
+Facilidad de ajuste: Se puede tallar y pulir fácilmente para lograr un acabado preciso.
+Versatilidad clínica: Apto para coronas, puentes provisionales, carillas, incrustaciones y onlays.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1736870874/Copia_de_DSCF3128-removebg-preview_qlhklo.png</t>
+  </si>
+  <si>
+    <t>RelyX™ Temp NE</t>
+  </si>
+  <si>
+    <t>RelyX™ Temp NE es un cemento dental temporal de alta calidad desarrollado por 3M ESPE. Este material está diseñado específicamente para la fijación temporal de restauraciones como coronas, puentes y otros elementos provisionales. Su fórmula a base de óxido de zinc sin eugenol elimina el riesgo de interferencias químicas con materiales restaurativos definitivos, como los cementos a base de resinas, garantizando un desempeño seguro y eficaz. Su manipulación es sencilla, lo que facilita su aplicación en el consultorio odontológico, y ofrece una resistencia adecuada para mantener restauraciones provisionales en su lugar durante el tiempo necesario.</t>
+  </si>
+  <si>
+    <t>Base: Óxido de zinc no eugenol.
+Incluye dos componentes: pasta base y pasta catalizadora.
+Presentación: tubo de 30 g (Pasta base) y 13 g (Pasta catalizadora).
+Propiedades: Fácil manipulación, tiempo adecuado de fraguado y resistencia suficiente para uso provisional.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1736873321/Copia_de_DSCF3147-removebg-preview_hceeec.png</t>
+  </si>
+  <si>
+    <t>3M™ Sof-Lex™ – Essential Kit</t>
+  </si>
+  <si>
+    <t>El kit 3M™ Sof-Lex™ es un sistema diseñado para realizar el pulido y contorneado de restauraciones dentales con alta precisión. Este set incluye discos flexibles y herramientas complementarias que permiten al odontólogo trabajar en superficies restaurativas, logrando un acabado suave y estético. Los discos permiten pulir y contornear materiales como resinas compuestas y otros restaurativos, ofreciendo un brillo natural y uniforme que imita el esmalte dental.</t>
+  </si>
+  <si>
+    <t>Contenido del kit: 4 tipos de discos Sof-Lex™ con diferentes granulometrías (grueso, mediano, fino y superfino), discos de diversos tamaños para áreas específicas de trabajo, mandril para montaje de discos.
+Fácil de usar: Los discos son fáciles de montar y desmontar en el mandril incluido.
+Adaptabilidad: Su diseño flexible permite trabajar en superficies curvas y zonas de difícil acceso.
+Diferentes granulometrías: Incluye discos que cubren desde el contorneado inicial hasta el pulido final.
+Resultados estéticos: Ofrece acabados suaves y brillantes, imitando el esmalte dental natural.
+Durabilidad: Material resistente al desgaste que garantiza un uso continuo sin pérdida de eficacia.
+Aplicación versátil: Apto para restauraciones de composite, resinas híbridas, microhíbridas y otros materiales.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1736876350/Captura_de_pantalla_2025-01-14_123825_xdchpj.png</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b val="0"/>
+        <color theme="1"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>Filtek</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b val="0"/>
+        <color theme="1"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>Z250 XT</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <b/>
+        <color theme="1"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <t>El 3M™ Filtek™ Z250 XT es un restaurador universal nanohíbrido diseñado para procedimientos restaurativos en odontología. Este material combina tecnología avanzada de resina y partículas nanométricas para ofrecer resistencia, estética y facilidad de manipulación. Es ideal para restauraciones directas en dientes anteriores y posteriores, garantizando un acabado natural y duradero.</t>
+  </si>
+  <si>
+    <t>Versatilidad: Diseñado para restauraciones en dientes anteriores y posteriores.
+Fácil manipulación: Posee una consistencia cremosa que facilita su aplicación y modelado.
+Alta resistencia: Ofrece durabilidad y resistencia al desgaste, ideal para zonas de alta carga masticatoria.
+Estética superior: Proporciona un acabado brillante y natural gracias a su capacidad para mimetizarse con el diente.
+Tonos variados: Disponible en múltiples tonos para adaptarse a diferentes necesidades estéticas.
+Tecnología nanohíbrida: Combina nanopartículas con rellenos tradicionales para mejorar la estética y la resistencia.
+Adherencia confiable: Compatible con diferentes adhesivos dentales para una unión segura y duradera.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1736883723/Restaurador_Universal_Nanoh%C3%ADbrido_3M_Filtek_Z250_XT_4_mtb3ud.png</t>
+    </r>
+  </si>
+  <si>
+    <t>Hybrilux Nano</t>
+  </si>
+  <si>
+    <t>El Hybrilux Nano de Densell es una resina compuesta nanohíbrida fotopolimerizable, diseñada para realizar restauraciones dentales directas en dientes anteriores y posteriores. Ofrece una estética superior, resistencia al desgaste y un manejo sencillo, lo que la convierte en una solución confiable para tratamientos restaurativos de alta calidad.</t>
+  </si>
+  <si>
+    <t>Aplicación universal: Apta para restauraciones en dientes anteriores y posteriores.
+Estética superior: Excelente mimetización con el diente natural gracias a su translucidez.
+Resistencia al desgaste: Ideal para zonas de alta carga masticatoria.
+Fácil manejo: Consistencia optimizada que facilita la colocación.</t>
+  </si>
+  <si>
+    <t>Densell</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1736865878/DSCF0180_copia__nzqnnj.png</t>
+    </r>
+  </si>
+  <si>
+    <t>MonoBond ET</t>
+  </si>
+  <si>
+    <t>El MonoBond ET de Densell es un adhesivo universal fotopolimerizable que garantiza una excelente adhesión al esmalte y dentina. Su versatilidad lo hace compatible con cualquier sistema de resina compuesta y puede usarse en técnicas de grabado total, autograbado o híbridas, ofreciendo resultados seguros y duraderos en procedimientos restaurativos.</t>
+  </si>
+  <si>
+    <t>Tipo: Adhesivo universal de fotocurado.
+Presentación: Frasco de 5 ml.
+Adhesión efectiva: Compatible con esmalte y dentina.
+Compatibilidad universal: Puede usarse con cualquier sistema de resina compuesta.
+Versatilidad: Apto para técnicas de grabado total, autograbado o híbridas.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1736865870/hibrilux_nano_jf31rk.png</t>
+    </r>
+  </si>
+  <si>
+    <t>Hybrilux Flow</t>
+  </si>
+  <si>
+    <t>Hybrilux Flow es una resina fluida fotopolimerizable diseñada por Densell para restauraciones dentales de alta precisión. Su fórmula combina partículas híbridas que le confieren resistencia mecánica, facilidad de aplicación y excelentes resultados estéticos. Es especialmente útil en cavidades pequeñas, zonas de difícil acceso, y como base para restauraciones compuestas.
+Ideal para casos de restauraciones de clases III y V, pequeñas cavidades de clase I, reparaciones de carillas y sellado de fisuras, Hybrilux Flow es una solución versátil y confiable en procedimientos restaurativos.</t>
+  </si>
+  <si>
+    <t>Composición híbrida avanzada: Combina partículas de relleno para alta resistencia mecánica y estética.
+Fotopolimerizable: Endurece rápidamente con luz de curado.
+Consistencia fluida: Fácil de aplicar en cavidades pequeñas y áreas difíciles de acceder.
+Variedad de tonos: Disponible en varios tonos para lograr una estética natural.
+Alta resistencia al desgaste: Prolonga la vida útil de las restauraciones.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1736881280/DSCF3198-removebg___u0lzux.png</t>
+  </si>
+  <si>
+    <t>Etching Gel</t>
+  </si>
+  <si>
+    <t>El Etching Gel de Densell es un gel grabador utilizado en odontología para acondicionar las superficies dentales antes de la aplicación de adhesivos y resinas. Está formulado con ácido fosfórico al 37%, lo que permite un grabado efectivo del esmalte y la dentina, garantizando una excelente adhesión mecánica entre el material restaurador y el tejido dental. Su textura en gel y color azul facilitan una aplicación controlada y precisa.</t>
+  </si>
+  <si>
+    <t>Composición efectiva: Contiene ácido fosfórico al 37%, garantizando un grabado eficiente.
+Textura en gel: Evita que el material se desplace, facilitando un control preciso durante su aplicación.
+Color azul brillante: Permite visualizar claramente dónde se aplica el producto.
+Fácil aplicación: Se presenta en jeringas que permiten una dispensación directa y sin desperdicio.
+Compatibilidad universal: Se puede usar con la mayoría de los adhesivos y resinas dentales.
+Grabado controlado: Proporciona una textura ideal para maximizar la adhesión mecánica.
+Seguro y eficaz: Diseñado para minimizar la sensibilidad dental cuando se usa correctamente.</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1736978418/Pica-enhance-20250115164907-removebg-preview_y18zgq.png</t>
+  </si>
+  <si>
+    <t>Glass Liner Base</t>
+  </si>
+  <si>
+    <t>El Glass Liner Base de Densell es un material de revestimiento para cavidades diseñado para proteger el tejido dental en procedimientos restaurativos. Actúa como una base o revestimiento que previene la microfiltración, protege contra agresiones químicas y proporciona un soporte ideal para restauraciones posteriores. Este producto es ideal para garantizar la durabilidad y la estabilidad de los materiales restaurativos, mejorando los resultados clínicos.</t>
+  </si>
+  <si>
+    <t>Propiedades protectoras: Forma una barrera efectiva contra ácidos y materiales irritantes.
+Compatibilidad: Funciona con diversos materiales restaurativos, como resinas compuestas y amalgamas.
+Fácil aplicación: Se presenta en jeringas, lo que permite un uso controlado y sin desperdicio.
+Baja solubilidad: Garantiza una mayor durabilidad y resistencia en el tiempo.
+Adherencia eficiente: Crea una unión fuerte con el tejido dental, reduciendo el riesgo de desprendimientos.
+Consistencia adecuada: Permite una manipulación fácil y uniforme en la cavidad dental.
+Versatilidad: Apto para diversas aplicaciones en restauraciones, como base o liner intermedio.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1736882702/pixelcut-export_2_s972w1.png</t>
+    </r>
+  </si>
+  <si>
+    <t>Coltosol Filling</t>
+  </si>
+  <si>
+    <t>El Coltosol Filling Densell es un material de obturación temporal diseñado para restauraciones provisionales en odontología. Este producto es fácil de manejar y aplicar, proporcionando un sellado efectivo y confiable para proteger la cavidad dental hasta que se realice el procedimiento definitivo.</t>
+  </si>
+  <si>
+    <t>Uso provisional: Diseñado específicamente para obturaciones temporales.
+Sellado efectivo: Proporciona una protección adecuada para evitar la entrada de contaminantes en la cavidad dental.
+Fácil de manejar: Posee una consistencia maleable que facilita su aplicación directa.
+Fraguado rápido: Endurece rápidamente en contacto con la humedad bucal.
+Biocompatible: Seguro para los tejidos dentales y orales.
+Presentación: Disponible en envase de 40 gramos, adecuado para múltiples aplicaciones.
+Versátil: Compatible con diferentes tipos de restauraciones temporales.
+Duradero: Mantiene su integridad estructural durante el período de uso temporal.</t>
+  </si>
+  <si>
+    <t>Eugenol x 20 ml</t>
+  </si>
+  <si>
+    <t>El Eugenol x 20 ml de Densell es un líquido de uso odontológico ampliamente utilizado como sedante dental y en la preparación de cementos temporales. Su acción calmante ayuda a aliviar el dolor en tratamientos de conducto y cavidades dentales. Es un producto esencial en consultorios dentales por su versatilidad y propiedades terapéuticas.</t>
+  </si>
+  <si>
+    <t>Función sedante: Reduce la sensibilidad y el dolor dental en tratamientos temporales.
+Uso en cementos temporales: Se mezcla con óxido de zinc para formar un cemento temporal eficaz.
+Propiedades antimicrobianas: Contribuye a la desinfección del área tratada.
+Presentación: Frasco de 20 ml, fácil de manejar y almacenar.
+Compatibilidad: Apto para usar en diversos procedimientos dentales.
+Efecto calmante: Ideal para tratamientos temporales, especialmente en casos de pulpitis o sensibilidad dental.
+Durabilidad: Producto estable y de larga duración cuando se almacena correctamente.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1736884835/6575-20_k6dyol.jpg</t>
+    </r>
+  </si>
+  <si>
+    <t>Guantes de Látex Blanco con Polvo</t>
+  </si>
+  <si>
+    <t>Guantes desechables fabricados en látex, diseñados para garantizar una barrera protectora eficiente. Incluyen polvo para facilitar su colocación y mejorar el confort durante su uso.</t>
+  </si>
+  <si>
+    <t>Material: Látex
+Color: Blanco
+Incluyen polvo
+Talla: M, L, XL
+Uso: Ideal para procedimientos odontológicos y médicos que requieren precisión y protección.</t>
+  </si>
+  <si>
+    <t>Gospa</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1736948506/Captura_de_pantalla_2025-01-15_083534-removebg-preview_pailr3.png</t>
+  </si>
+  <si>
+    <t>Guantes de Látex Sin Polvo</t>
+  </si>
+  <si>
+    <t>Guantes desechables de látex sin polvo, diseñados para personas con sensibilidad a este componente. Proporcionan máxima protección y comodidad durante el uso.</t>
+  </si>
+  <si>
+    <t>Material: Látex
+Color: Blanco
+Sin polvo
+Talla: XS, S, M, L 
+Uso: Recomendado para procedimientos de examen y trabajos odontológicos.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>https://res.cloudinary.com/diqmtzief/image/upload/v1736948500/Captura_de_pantalla_2025-01-15_083416-removebg-preview_ygdgct.png</t>
+    </r>
+  </si>
+  <si>
+    <t>Unidad Dental con Sillón Integrado</t>
+  </si>
+  <si>
+    <t>Equipo odontológico multifuncional diseñado para procedimientos clínicos y restaurativos. Incluye un sillón ergonómico con tapizado en color rojo, lámpara dental LED, bandeja de instrumentos y monitor integrado. Ideal para clínicas odontológicas que buscan comodidad, funcionalidad y tecnología avanzada en un solo dispositivo.</t>
+  </si>
+  <si>
+    <t>Sillón: Tapizado en cuero sintético rojo, ajustable para diversas posiciones, con soporte lumbar.
+Lámpara dental: LED de alta intensidad, con ajuste de posición para mejorar la visibilidad.
+Monitor: Pantalla integrada para visualizar radiografías o imágenes clínicas.
+Bandeja de instrumentos: Incluye soporte para herramientas odontológicas con conectores de alta y baja velocidad.
+Pieza de mano: Opciones de conexión para diversas funciones clínicas.
+Pedal: Control eléctrico con múltiples configuraciones.
+Material: Estructura robusta de acero inoxidable y plástico ABS.
+Uso: Procedimientos odontológicos de diagnóstico, ortodoncia y restaurativos.</t>
+  </si>
+  <si>
+    <t>Equipos</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/diqmtzief/image/upload/v1736949710/DSCF6634_gcczg4.jpg</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1373,6 +1833,13 @@
       <u/>
       <color rgb="FF0000FF"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -1568,7 +2035,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1635,13 +2102,19 @@
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="8" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="12" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -1702,8 +2175,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I73" displayName="Productos" name="Productos" id="1">
-  <autoFilter ref="$A$1:$I$73"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:I93" displayName="Productos" name="Productos" id="1">
+  <autoFilter ref="$A$1:$I$93"/>
   <tableColumns count="9">
     <tableColumn name="id" id="1"/>
     <tableColumn name="nombre" id="2"/>
@@ -3831,29 +4304,547 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="22">
+      <c r="A73" s="20">
         <v>72.0</v>
       </c>
-      <c r="B73" s="23" t="s">
+      <c r="B73" s="11" t="s">
         <v>293</v>
       </c>
-      <c r="C73" s="23" t="s">
+      <c r="C73" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="D73" s="23" t="s">
+      <c r="D73" s="11" t="s">
         <v>294</v>
       </c>
-      <c r="E73" s="23" t="s">
+      <c r="E73" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F73" s="23" t="s">
+      <c r="F73" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="G73" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="I73" s="24" t="s">
+      <c r="G73" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I73" s="17" t="s">
         <v>295</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="21">
+        <v>73.0</v>
+      </c>
+      <c r="B74" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="C74" s="14" t="s">
+        <v>297</v>
+      </c>
+      <c r="D74" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="E74" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F74" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="G74" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I74" s="16" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="20">
+        <v>74.0</v>
+      </c>
+      <c r="B75" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="C75" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="D75" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="E75" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F75" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="G75" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I75" s="13" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="21">
+        <v>75.0</v>
+      </c>
+      <c r="B76" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="C76" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="D76" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="E76" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F76" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="G76" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I76" s="8" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="20">
+        <v>76.0</v>
+      </c>
+      <c r="B77" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="C77" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="D77" s="11" t="s">
+        <v>311</v>
+      </c>
+      <c r="E77" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F77" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="G77" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I77" s="13" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="21">
+        <v>77.0</v>
+      </c>
+      <c r="B78" s="14" t="s">
+        <v>313</v>
+      </c>
+      <c r="C78" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="D78" s="14" t="s">
+        <v>315</v>
+      </c>
+      <c r="E78" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F78" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="G78" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I78" s="16" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="20">
+        <v>78.0</v>
+      </c>
+      <c r="B79" s="11" t="s">
+        <v>317</v>
+      </c>
+      <c r="C79" s="11" t="s">
+        <v>318</v>
+      </c>
+      <c r="D79" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="E79" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F79" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="G79" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I79" s="13" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="21">
+        <v>79.0</v>
+      </c>
+      <c r="B80" s="14" t="s">
+        <v>321</v>
+      </c>
+      <c r="C80" s="14" t="s">
+        <v>322</v>
+      </c>
+      <c r="D80" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="E80" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F80" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="G80" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I80" s="19" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="20">
+        <v>80.0</v>
+      </c>
+      <c r="B81" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="C81" s="11" t="s">
+        <v>326</v>
+      </c>
+      <c r="D81" s="11" t="s">
+        <v>327</v>
+      </c>
+      <c r="E81" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F81" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="G81" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I81" s="17" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="21">
+        <v>81.0</v>
+      </c>
+      <c r="B82" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="C82" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="D82" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="E82" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F82" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="G82" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I82" s="16" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="20">
+        <v>82.0</v>
+      </c>
+      <c r="B83" s="22" t="s">
+        <v>333</v>
+      </c>
+      <c r="C83" s="11" t="s">
+        <v>334</v>
+      </c>
+      <c r="D83" s="11" t="s">
+        <v>335</v>
+      </c>
+      <c r="E83" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F83" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="G83" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I83" s="13" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="21">
+        <v>83.0</v>
+      </c>
+      <c r="B84" s="14" t="s">
+        <v>337</v>
+      </c>
+      <c r="C84" s="14" t="s">
+        <v>338</v>
+      </c>
+      <c r="D84" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="E84" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F84" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="G84" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I84" s="16" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="20">
+        <v>84.0</v>
+      </c>
+      <c r="B85" s="11" t="s">
+        <v>342</v>
+      </c>
+      <c r="C85" s="11" t="s">
+        <v>343</v>
+      </c>
+      <c r="D85" s="11" t="s">
+        <v>344</v>
+      </c>
+      <c r="E85" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F85" s="11" t="s">
+        <v>340</v>
+      </c>
+      <c r="G85" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I85" s="13" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="21">
+        <v>85.0</v>
+      </c>
+      <c r="B86" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="C86" s="14" t="s">
+        <v>347</v>
+      </c>
+      <c r="D86" s="14" t="s">
+        <v>348</v>
+      </c>
+      <c r="E86" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F86" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="G86" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I86" s="19" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="20">
+        <v>86.0</v>
+      </c>
+      <c r="B87" s="11" t="s">
+        <v>350</v>
+      </c>
+      <c r="C87" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="D87" s="11" t="s">
+        <v>352</v>
+      </c>
+      <c r="E87" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F87" s="11" t="s">
+        <v>340</v>
+      </c>
+      <c r="G87" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I87" s="17" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="21">
+        <v>87.0</v>
+      </c>
+      <c r="B88" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="C88" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="D88" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="E88" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F88" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="G88" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I88" s="16" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="20">
+        <v>88.0</v>
+      </c>
+      <c r="B89" s="11" t="s">
+        <v>358</v>
+      </c>
+      <c r="C89" s="11" t="s">
+        <v>359</v>
+      </c>
+      <c r="D89" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="E89" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F89" s="11" t="s">
+        <v>340</v>
+      </c>
+      <c r="G89" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I89" s="23"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="21">
+        <v>89.0</v>
+      </c>
+      <c r="B90" s="14" t="s">
+        <v>361</v>
+      </c>
+      <c r="C90" s="14" t="s">
+        <v>362</v>
+      </c>
+      <c r="D90" s="14" t="s">
+        <v>363</v>
+      </c>
+      <c r="E90" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F90" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="G90" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I90" s="16" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="20">
+        <v>90.0</v>
+      </c>
+      <c r="B91" s="11" t="s">
+        <v>365</v>
+      </c>
+      <c r="C91" s="11" t="s">
+        <v>366</v>
+      </c>
+      <c r="D91" s="11" t="s">
+        <v>367</v>
+      </c>
+      <c r="E91" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F91" s="11" t="s">
+        <v>368</v>
+      </c>
+      <c r="G91" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I91" s="17" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="21">
+        <v>91.0</v>
+      </c>
+      <c r="B92" s="14" t="s">
+        <v>370</v>
+      </c>
+      <c r="C92" s="14" t="s">
+        <v>371</v>
+      </c>
+      <c r="D92" s="14" t="s">
+        <v>372</v>
+      </c>
+      <c r="E92" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F92" s="14" t="s">
+        <v>368</v>
+      </c>
+      <c r="G92" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I92" s="16" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="24">
+        <v>92.0</v>
+      </c>
+      <c r="B93" s="25" t="s">
+        <v>374</v>
+      </c>
+      <c r="C93" s="25" t="s">
+        <v>375</v>
+      </c>
+      <c r="D93" s="25" t="s">
+        <v>376</v>
+      </c>
+      <c r="E93" s="25" t="s">
+        <v>377</v>
+      </c>
+      <c r="F93" s="25" t="s">
+        <v>368</v>
+      </c>
+      <c r="G93" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="I93" s="26" t="s">
+        <v>378</v>
       </c>
     </row>
   </sheetData>
@@ -3930,10 +4921,29 @@
     <hyperlink r:id="rId70" ref="I71"/>
     <hyperlink r:id="rId71" ref="I72"/>
     <hyperlink r:id="rId72" ref="I73"/>
+    <hyperlink r:id="rId73" ref="I74"/>
+    <hyperlink r:id="rId74" ref="I75"/>
+    <hyperlink r:id="rId75" ref="I76"/>
+    <hyperlink r:id="rId76" ref="I77"/>
+    <hyperlink r:id="rId77" ref="I78"/>
+    <hyperlink r:id="rId78" ref="I79"/>
+    <hyperlink r:id="rId79" ref="I80"/>
+    <hyperlink r:id="rId80" ref="I81"/>
+    <hyperlink r:id="rId81" ref="I82"/>
+    <hyperlink r:id="rId82" ref="I83"/>
+    <hyperlink r:id="rId83" ref="I84"/>
+    <hyperlink r:id="rId84" ref="I85"/>
+    <hyperlink r:id="rId85" ref="I86"/>
+    <hyperlink r:id="rId86" ref="I87"/>
+    <hyperlink r:id="rId87" ref="I88"/>
+    <hyperlink r:id="rId88" ref="I90"/>
+    <hyperlink r:id="rId89" ref="I91"/>
+    <hyperlink r:id="rId90" ref="I92"/>
+    <hyperlink r:id="rId91" ref="I93"/>
   </hyperlinks>
-  <drawing r:id="rId73"/>
+  <drawing r:id="rId92"/>
   <tableParts count="1">
-    <tablePart r:id="rId75"/>
+    <tablePart r:id="rId94"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>